<commit_message>
Updated vehicles - cannot shoot while in the vehicle EXCEPT the APC, which shoots machine guns!
</commit_message>
<xml_diff>
--- a/gun infos.xlsx
+++ b/gun infos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E507B2DE-4933-4ACA-BF03-3A34777836A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E060E1-C8EA-46F9-AF33-791A75CBEF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29810" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14670" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1298,7 +1298,7 @@
   <dimension ref="A1:AH45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2729,7 +2729,7 @@
         <v>0.5</v>
       </c>
       <c r="F23" s="23">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G23" s="23">
         <v>17</v>
@@ -2746,7 +2746,7 @@
       <c r="K23" s="23"/>
       <c r="L23" s="23">
         <f>ROUND(D23*E23/F23*1000,2)</f>
-        <v>10</v>
+        <v>12.5</v>
       </c>
       <c r="M23" s="23">
         <f>ROUND(D23*E23/(F23+I23)*1000,2)</f>
@@ -3285,48 +3285,48 @@
         <v>74</v>
       </c>
       <c r="B43" s="45">
-        <f t="shared" ref="B43:L43" si="8">(2+B42)*tilesize+tilesize/2</f>
-        <v>192</v>
+        <f>(2+B42)*tilesize</f>
+        <v>128</v>
       </c>
       <c r="C43" s="45">
-        <f t="shared" si="8"/>
-        <v>320</v>
+        <f>(2+C42)*tilesize</f>
+        <v>256</v>
       </c>
       <c r="D43" s="45">
-        <f t="shared" si="8"/>
-        <v>448</v>
+        <f>(2+D42)*tilesize</f>
+        <v>384</v>
       </c>
       <c r="E43" s="45">
-        <f t="shared" si="8"/>
-        <v>576</v>
+        <f>(2+E42)*tilesize</f>
+        <v>512</v>
       </c>
       <c r="F43" s="45">
-        <f t="shared" si="8"/>
-        <v>704</v>
+        <f>(2+F42)*tilesize</f>
+        <v>640</v>
       </c>
       <c r="G43" s="45">
-        <f t="shared" si="8"/>
-        <v>832</v>
+        <f>(2+G42)*tilesize</f>
+        <v>768</v>
       </c>
       <c r="H43" s="45">
-        <f t="shared" si="8"/>
-        <v>960</v>
+        <f>(2+H42)*tilesize</f>
+        <v>896</v>
       </c>
       <c r="I43" s="45">
-        <f t="shared" si="8"/>
-        <v>1088</v>
+        <f>(2+I42)*tilesize</f>
+        <v>1024</v>
       </c>
       <c r="J43" s="45">
-        <f t="shared" si="8"/>
-        <v>1216</v>
+        <f>(2+J42)*tilesize</f>
+        <v>1152</v>
       </c>
       <c r="K43" s="45">
-        <f t="shared" si="8"/>
-        <v>1344</v>
+        <f>(2+K42)*tilesize</f>
+        <v>1280</v>
       </c>
       <c r="L43" s="45">
-        <f t="shared" si="8"/>
-        <v>1472</v>
+        <f>(2+L42)*tilesize</f>
+        <v>1408</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.45">
@@ -3334,47 +3334,47 @@
         <v>75</v>
       </c>
       <c r="B44" s="57">
-        <f t="shared" ref="B44:L44" si="9">(2+B42+1)*tilesize+tilesize/2</f>
+        <f t="shared" ref="B44:L44" si="8">(2+B42+1)*tilesize+tilesize/2</f>
         <v>320</v>
       </c>
       <c r="C44" s="58">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>448</v>
       </c>
       <c r="D44" s="59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>576</v>
       </c>
       <c r="E44" s="60">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>704</v>
       </c>
       <c r="F44" s="61">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>832</v>
       </c>
       <c r="G44" s="62">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>960</v>
       </c>
       <c r="H44" s="63">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1088</v>
       </c>
       <c r="I44" s="64">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1216</v>
       </c>
       <c r="J44" s="65">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1344</v>
       </c>
       <c r="K44" s="66">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1472</v>
       </c>
       <c r="L44" s="67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1600</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New weapon: tank buster
</commit_message>
<xml_diff>
--- a/gun infos.xlsx
+++ b/gun infos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E060E1-C8EA-46F9-AF33-791A75CBEF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B67987-2B66-4099-BCF8-3ED46E411904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14670" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="0" windowWidth="31240" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="90">
   <si>
     <t>Weapon info</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -403,12 +403,24 @@
     <t>Some constants</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>tank buster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rocket</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Designed to destroy a tank (too slow bullet for practical fights)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -518,13 +530,6 @@
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -811,7 +816,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -901,34 +906,30 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -959,26 +960,29 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -994,9 +998,6 @@
     <xf numFmtId="0" fontId="26" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1007,10 +1008,10 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1298,7 +1299,7 @@
   <dimension ref="A1:AH45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1407,7 +1408,7 @@
       <c r="A3" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="59">
+      <c r="B3" s="57">
         <v>576</v>
       </c>
       <c r="C3" s="24">
@@ -1454,15 +1455,15 @@
         <v>0.9</v>
       </c>
       <c r="P3" s="23">
-        <f t="shared" ref="P3:P4" si="0">-(FLOOR(G3/6,1)-1)</f>
+        <f t="shared" ref="P3:P5" si="0">-(FLOOR(G3/6,1)-1)</f>
         <v>-1</v>
       </c>
       <c r="Q3" s="23">
-        <f t="shared" ref="Q3:Q4" si="1">ROUND(C3/G3,3)</f>
+        <f t="shared" ref="Q3:Q5" si="1">ROUND(C3/G3,3)</f>
         <v>0</v>
       </c>
-      <c r="R3" s="30" t="s">
-        <v>81</v>
+      <c r="R3" s="26" t="s">
+        <v>30</v>
       </c>
       <c r="S3" s="23"/>
       <c r="T3" s="23">
@@ -1485,17 +1486,17 @@
       <c r="Y3" t="s">
         <v>77</v>
       </c>
-      <c r="AF3" s="71" t="s">
+      <c r="AF3" s="69" t="s">
         <v>78</v>
       </c>
-      <c r="AG3" s="54"/>
-      <c r="AH3" s="54"/>
+      <c r="AG3" s="52"/>
+      <c r="AH3" s="52"/>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A4" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="69">
+      <c r="B4" s="67">
         <v>192</v>
       </c>
       <c r="C4" s="28">
@@ -1535,7 +1536,7 @@
         <f>D4*E4*H4</f>
         <v>10</v>
       </c>
-      <c r="O4" s="41">
+      <c r="O4" s="39">
         <f>ROUND(playerHealth/(D4*E4),1)</f>
         <v>4</v>
       </c>
@@ -1547,15 +1548,15 @@
         <f t="shared" si="1"/>
         <v>0.375</v>
       </c>
-      <c r="R4" s="40" t="s">
+      <c r="R4" s="38" t="s">
         <v>80</v>
       </c>
       <c r="S4" s="28"/>
       <c r="T4" s="23">
-        <f t="shared" ref="T4" si="2" xml:space="preserve"> D4*E4*7/10</f>
+        <f t="shared" ref="T4:T5" si="2" xml:space="preserve"> D4*E4*7/10</f>
         <v>1.4</v>
       </c>
-      <c r="U4" s="42">
+      <c r="U4" s="40">
         <f>ROUND(playerHealth/(T4),2)</f>
         <v>5.71</v>
       </c>
@@ -1573,38 +1574,96 @@
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A5" s="22"/>
-      <c r="B5" s="68"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="33"/>
+      <c r="A5" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="59">
+        <v>832</v>
+      </c>
+      <c r="C5" s="23">
+        <v>0</v>
+      </c>
+      <c r="D5" s="24">
+        <v>1</v>
+      </c>
+      <c r="E5" s="23">
+        <v>200</v>
+      </c>
+      <c r="F5" s="23">
+        <v>4000</v>
+      </c>
+      <c r="G5" s="23">
+        <v>6</v>
+      </c>
+      <c r="H5" s="23">
+        <v>1</v>
+      </c>
+      <c r="I5" s="23">
+        <v>6000</v>
+      </c>
+      <c r="J5" s="28" t="s">
+        <v>88</v>
+      </c>
       <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="40"/>
+      <c r="L5" s="23">
+        <f t="shared" ref="L5" si="4">ROUND(D5*E5/F5*1000,2)</f>
+        <v>50</v>
+      </c>
+      <c r="M5" s="23">
+        <f t="shared" ref="M5" si="5">ROUND(D5*E5/(F5+I5)*1000,2)</f>
+        <v>20</v>
+      </c>
+      <c r="N5" s="23">
+        <f t="shared" ref="N5" si="6">D5*E5*H5</f>
+        <v>200</v>
+      </c>
+      <c r="O5" s="29">
+        <f>ROUND(playerHealth/(D5*E5),1)</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="30" t="s">
+        <v>81</v>
+      </c>
       <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="35"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="31"/>
+      <c r="T5" s="23">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+      <c r="U5" s="32">
+        <f>ROUND(playerHealth/(T5),2)</f>
+        <v>0.06</v>
+      </c>
+      <c r="V5" s="23">
+        <f t="shared" si="3"/>
+        <v>199.6</v>
+      </c>
+      <c r="W5" s="32">
+        <f>ROUND(playerHealth/(V5),2)</f>
+        <v>0.04</v>
+      </c>
       <c r="X5" s="23"/>
+      <c r="Y5" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="B6" s="70"/>
-      <c r="O6" s="37"/>
+      <c r="B6" s="68"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="36"/>
       <c r="P6" s="23"/>
       <c r="Q6" s="23"/>
       <c r="T6" s="23"/>
-      <c r="U6" s="35"/>
+      <c r="U6" s="34"/>
       <c r="V6" s="23"/>
       <c r="W6" s="31"/>
     </row>
@@ -1612,7 +1671,7 @@
       <c r="A7" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="66">
+      <c r="B7" s="64">
         <v>1472</v>
       </c>
       <c r="C7" s="23">
@@ -1652,7 +1711,7 @@
         <f>D7*E7*H7</f>
         <v>25</v>
       </c>
-      <c r="O7" s="38">
+      <c r="O7" s="36">
         <f>ROUND(playerHealth/(D7*E7),1)</f>
         <v>1.6</v>
       </c>
@@ -1672,7 +1731,7 @@
         <f xml:space="preserve"> D7*E7*7/10</f>
         <v>3.5</v>
       </c>
-      <c r="U7" s="35">
+      <c r="U7" s="34">
         <f>ROUND(playerHealth/(T7),2)</f>
         <v>2.29</v>
       </c>
@@ -1690,7 +1749,7 @@
       <c r="A8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="63">
+      <c r="B8" s="61">
         <v>1088</v>
       </c>
       <c r="C8" s="23">
@@ -1742,15 +1801,15 @@
         <f>ROUND(C8/G8,3)</f>
         <v>3.1E-2</v>
       </c>
-      <c r="R8" s="34" t="s">
+      <c r="R8" s="33" t="s">
         <v>31</v>
       </c>
       <c r="S8" s="23"/>
       <c r="T8" s="23">
-        <f t="shared" ref="T8:T23" si="4" xml:space="preserve"> D8*E8*9/10</f>
+        <f t="shared" ref="T8:T23" si="7" xml:space="preserve"> D8*E8*9/10</f>
         <v>2.7</v>
       </c>
-      <c r="U8" s="35">
+      <c r="U8" s="34">
         <f>ROUND(playerHealth/(T8),2)</f>
         <v>2.96</v>
       </c>
@@ -1758,7 +1817,7 @@
         <f t="shared" si="3"/>
         <v>2.6</v>
       </c>
-      <c r="W8" s="36">
+      <c r="W8" s="35">
         <f>ROUND(playerHealth/(V8),2)</f>
         <v>3.08</v>
       </c>
@@ -1768,7 +1827,7 @@
       <c r="A9" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="64">
+      <c r="B9" s="62">
         <v>1216</v>
       </c>
       <c r="C9" s="23">
@@ -1820,7 +1879,7 @@
         <f>ROUND(C9/G9,3)</f>
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="R9" s="34" t="s">
+      <c r="R9" s="33" t="s">
         <v>31</v>
       </c>
       <c r="S9" s="23"/>
@@ -1828,7 +1887,7 @@
         <f xml:space="preserve"> D9*E9*7/10</f>
         <v>2.4500000000000002</v>
       </c>
-      <c r="U9" s="36">
+      <c r="U9" s="35">
         <f>ROUND(playerHealth/(T9),2)</f>
         <v>3.27</v>
       </c>
@@ -1836,7 +1895,7 @@
         <f t="shared" si="3"/>
         <v>3.1</v>
       </c>
-      <c r="W9" s="35">
+      <c r="W9" s="34">
         <f>ROUND(playerHealth/(V9),2)</f>
         <v>2.58</v>
       </c>
@@ -1846,7 +1905,7 @@
       <c r="A10" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="67">
+      <c r="B10" s="65">
         <v>1600</v>
       </c>
       <c r="C10" s="23">
@@ -1924,8 +1983,8 @@
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A11" s="39"/>
-      <c r="B11" s="68"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="66"/>
       <c r="C11" s="23"/>
       <c r="D11" s="28"/>
       <c r="E11" s="23"/>
@@ -1941,19 +2000,19 @@
       <c r="O11" s="25"/>
       <c r="P11" s="23"/>
       <c r="Q11" s="23"/>
-      <c r="R11" s="40"/>
+      <c r="R11" s="38"/>
       <c r="S11" s="23"/>
       <c r="T11" s="23"/>
-      <c r="U11" s="35"/>
+      <c r="U11" s="34"/>
       <c r="V11" s="23"/>
-      <c r="W11" s="35"/>
+      <c r="W11" s="34"/>
       <c r="X11" s="23"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A12" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="59">
+      <c r="B12" s="57">
         <v>576</v>
       </c>
       <c r="C12" s="23">
@@ -1993,7 +2052,7 @@
         <f>D12*E12*H12</f>
         <v>15</v>
       </c>
-      <c r="O12" s="41">
+      <c r="O12" s="39">
         <f>ROUND(playerHealth/(D12*E12),1)</f>
         <v>8</v>
       </c>
@@ -2005,15 +2064,15 @@
         <f>ROUND(C12/G12,3)</f>
         <v>0.2</v>
       </c>
-      <c r="R12" s="34" t="s">
+      <c r="R12" s="33" t="s">
         <v>31</v>
       </c>
       <c r="S12" s="23"/>
       <c r="T12" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.9</v>
       </c>
-      <c r="U12" s="42">
+      <c r="U12" s="40">
         <f>ROUND(playerHealth/(T12),2)</f>
         <v>8.89</v>
       </c>
@@ -2021,7 +2080,7 @@
         <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
-      <c r="W12" s="42">
+      <c r="W12" s="40">
         <f>ROUND(playerHealth/(V12),2)</f>
         <v>13.33</v>
       </c>
@@ -2031,7 +2090,7 @@
       <c r="A13" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="61">
+      <c r="B13" s="59">
         <v>832</v>
       </c>
       <c r="C13" s="23">
@@ -2071,7 +2130,7 @@
         <f>D13*E13*H13</f>
         <v>150</v>
       </c>
-      <c r="O13" s="41">
+      <c r="O13" s="39">
         <f>ROUND(playerHealth/(D13*E13),1)</f>
         <v>8</v>
       </c>
@@ -2088,10 +2147,10 @@
       </c>
       <c r="S13" s="23"/>
       <c r="T13" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.9</v>
       </c>
-      <c r="U13" s="42">
+      <c r="U13" s="40">
         <f>ROUND(playerHealth/(T13),2)</f>
         <v>8.89</v>
       </c>
@@ -2099,7 +2158,7 @@
         <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
-      <c r="W13" s="42">
+      <c r="W13" s="40">
         <f>ROUND(playerHealth/(V13),2)</f>
         <v>13.33</v>
       </c>
@@ -2112,7 +2171,7 @@
       <c r="A14" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="63">
+      <c r="B14" s="61">
         <v>1088</v>
       </c>
       <c r="C14" s="23">
@@ -2152,7 +2211,7 @@
         <f>D14*E14*H14</f>
         <v>10</v>
       </c>
-      <c r="O14" s="41">
+      <c r="O14" s="39">
         <f>ROUND(playerHealth/(D14*E14),1)</f>
         <v>8</v>
       </c>
@@ -2169,10 +2228,10 @@
       </c>
       <c r="S14" s="23"/>
       <c r="T14" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.9</v>
       </c>
-      <c r="U14" s="42">
+      <c r="U14" s="40">
         <f>ROUND(playerHealth/(T14),2)</f>
         <v>8.89</v>
       </c>
@@ -2180,7 +2239,7 @@
         <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
-      <c r="W14" s="42">
+      <c r="W14" s="40">
         <f>ROUND(playerHealth/(V14),2)</f>
         <v>13.33</v>
       </c>
@@ -2193,7 +2252,7 @@
       <c r="A15" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="60">
+      <c r="B15" s="58">
         <v>704</v>
       </c>
       <c r="C15" s="23">
@@ -2233,7 +2292,7 @@
         <f>D15*E15*H15</f>
         <v>30</v>
       </c>
-      <c r="O15" s="41">
+      <c r="O15" s="39">
         <f>ROUND(playerHealth/(D15*E15),1)</f>
         <v>8</v>
       </c>
@@ -2245,15 +2304,15 @@
         <f>ROUND(C15/G15,3)</f>
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="R15" s="34" t="s">
+      <c r="R15" s="33" t="s">
         <v>31</v>
       </c>
       <c r="S15" s="23"/>
       <c r="T15" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.9</v>
       </c>
-      <c r="U15" s="42">
+      <c r="U15" s="40">
         <f>ROUND(playerHealth/(T15),2)</f>
         <v>8.89</v>
       </c>
@@ -2261,7 +2320,7 @@
         <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
-      <c r="W15" s="42">
+      <c r="W15" s="40">
         <f>ROUND(playerHealth/(V15),2)</f>
         <v>13.33</v>
       </c>
@@ -2271,7 +2330,7 @@
       <c r="A16" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="59">
+      <c r="B16" s="57">
         <v>576</v>
       </c>
       <c r="C16" s="23">
@@ -2311,7 +2370,7 @@
         <f>D16*E16*H16</f>
         <v>30</v>
       </c>
-      <c r="O16" s="41">
+      <c r="O16" s="39">
         <f>ROUND(playerHealth/(D16*E16),1)</f>
         <v>8</v>
       </c>
@@ -2323,15 +2382,15 @@
         <f>ROUND(C16/G16,3)</f>
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="R16" s="34" t="s">
+      <c r="R16" s="33" t="s">
         <v>31</v>
       </c>
       <c r="S16" s="23"/>
       <c r="T16" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.9</v>
       </c>
-      <c r="U16" s="42">
+      <c r="U16" s="40">
         <f>ROUND(playerHealth/(T16),2)</f>
         <v>8.89</v>
       </c>
@@ -2339,7 +2398,7 @@
         <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
-      <c r="W16" s="42">
+      <c r="W16" s="40">
         <f>ROUND(playerHealth/(V16),2)</f>
         <v>13.33</v>
       </c>
@@ -2347,7 +2406,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A17" s="22"/>
-      <c r="B17" s="68"/>
+      <c r="B17" s="66"/>
       <c r="C17" s="23"/>
       <c r="D17" s="28"/>
       <c r="E17" s="23"/>
@@ -2363,19 +2422,19 @@
       <c r="O17" s="25"/>
       <c r="P17" s="23"/>
       <c r="Q17" s="23"/>
-      <c r="R17" s="40"/>
+      <c r="R17" s="38"/>
       <c r="S17" s="23"/>
       <c r="T17" s="23"/>
-      <c r="U17" s="35"/>
+      <c r="U17" s="34"/>
       <c r="V17" s="23"/>
-      <c r="W17" s="35"/>
+      <c r="W17" s="34"/>
       <c r="X17" s="23"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A18" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="57">
+      <c r="B18" s="55">
         <v>320</v>
       </c>
       <c r="C18" s="23">
@@ -2415,7 +2474,7 @@
         <f>D18*E18*H18</f>
         <v>10</v>
       </c>
-      <c r="O18" s="38">
+      <c r="O18" s="36">
         <f>ROUND(playerHealth/(D18*E18),1)</f>
         <v>1.6</v>
       </c>
@@ -2427,12 +2486,12 @@
         <f>ROUND(C18/G18,3)</f>
         <v>0.5</v>
       </c>
-      <c r="R18" s="34" t="s">
+      <c r="R18" s="33" t="s">
         <v>31</v>
       </c>
       <c r="S18" s="23"/>
       <c r="T18" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>4.5</v>
       </c>
       <c r="U18" s="31">
@@ -2443,7 +2502,7 @@
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="W18" s="35">
+      <c r="W18" s="34">
         <f>ROUND(playerHealth/(V18),2)</f>
         <v>2.67</v>
       </c>
@@ -2456,7 +2515,7 @@
       <c r="A19" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="58">
+      <c r="B19" s="56">
         <v>448</v>
       </c>
       <c r="C19" s="23">
@@ -2513,10 +2572,10 @@
       </c>
       <c r="S19" s="23"/>
       <c r="T19" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2.7</v>
       </c>
-      <c r="U19" s="35">
+      <c r="U19" s="34">
         <f>ROUND(playerHealth/(T19),2)</f>
         <v>2.96</v>
       </c>
@@ -2524,7 +2583,7 @@
         <f t="shared" si="3"/>
         <v>1.7999999999999998</v>
       </c>
-      <c r="W19" s="42">
+      <c r="W19" s="40">
         <f>ROUND(playerHealth/(V19),2)</f>
         <v>4.4400000000000004</v>
       </c>
@@ -2534,7 +2593,7 @@
       <c r="A20" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="58">
+      <c r="B20" s="56">
         <v>448</v>
       </c>
       <c r="C20" s="23">
@@ -2574,7 +2633,7 @@
         <f>D20*E20*H20</f>
         <v>10</v>
       </c>
-      <c r="O20" s="41">
+      <c r="O20" s="39">
         <f>ROUND(playerHealth/(D20*E20),1)</f>
         <v>4</v>
       </c>
@@ -2586,15 +2645,15 @@
         <f>ROUND(C20/G20,3)</f>
         <v>0.214</v>
       </c>
-      <c r="R20" s="34" t="s">
+      <c r="R20" s="33" t="s">
         <v>31</v>
       </c>
       <c r="S20" s="23"/>
       <c r="T20" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.8</v>
       </c>
-      <c r="U20" s="42">
+      <c r="U20" s="40">
         <f>ROUND(playerHealth/(T20),2)</f>
         <v>4.4400000000000004</v>
       </c>
@@ -2602,7 +2661,7 @@
         <f t="shared" si="3"/>
         <v>1.2</v>
       </c>
-      <c r="W20" s="42">
+      <c r="W20" s="40">
         <f>ROUND(playerHealth/(V20),2)</f>
         <v>6.67</v>
       </c>
@@ -2610,7 +2669,7 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A21" s="22"/>
-      <c r="B21" s="68"/>
+      <c r="B21" s="66"/>
       <c r="C21" s="23"/>
       <c r="D21" s="28"/>
       <c r="E21" s="23"/>
@@ -2626,19 +2685,19 @@
       <c r="O21" s="25"/>
       <c r="P21" s="23"/>
       <c r="Q21" s="23"/>
-      <c r="R21" s="40"/>
+      <c r="R21" s="38"/>
       <c r="S21" s="23"/>
       <c r="T21" s="23"/>
-      <c r="U21" s="35"/>
+      <c r="U21" s="34"/>
       <c r="V21" s="23"/>
-      <c r="W21" s="35"/>
+      <c r="W21" s="34"/>
       <c r="X21" s="23"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A22" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="68">
+      <c r="B22" s="66">
         <v>700</v>
       </c>
       <c r="C22" s="23">
@@ -2678,7 +2737,7 @@
         <f>D22*E22*H22</f>
         <v>12.5</v>
       </c>
-      <c r="O22" s="41">
+      <c r="O22" s="39">
         <f>ROUND(playerHealth/(D22*E22),1)</f>
         <v>16</v>
       </c>
@@ -2690,15 +2749,15 @@
         <f>ROUND(C22/G22,3)</f>
         <v>0.13300000000000001</v>
       </c>
-      <c r="R22" s="34" t="s">
+      <c r="R22" s="33" t="s">
         <v>31</v>
       </c>
       <c r="S22" s="23"/>
       <c r="T22" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.45</v>
       </c>
-      <c r="U22" s="42">
+      <c r="U22" s="40">
         <f>ROUND(playerHealth/(T22),2)</f>
         <v>17.78</v>
       </c>
@@ -2706,7 +2765,7 @@
         <f>D22*(E22-0.2)</f>
         <v>0.3</v>
       </c>
-      <c r="W22" s="42">
+      <c r="W22" s="40">
         <f>ROUND(playerHealth/(V22),2)</f>
         <v>26.67</v>
       </c>
@@ -2716,7 +2775,7 @@
       <c r="A23" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="68">
+      <c r="B23" s="66">
         <v>600</v>
       </c>
       <c r="C23" s="23">
@@ -2756,7 +2815,7 @@
         <f>D23*E23*H23</f>
         <v>9.5</v>
       </c>
-      <c r="O23" s="41">
+      <c r="O23" s="39">
         <f>ROUND(playerHealth/(D23*E23),1)</f>
         <v>16</v>
       </c>
@@ -2768,15 +2827,15 @@
         <f>ROUND(C23/G23,3)</f>
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="R23" s="34" t="s">
+      <c r="R23" s="33" t="s">
         <v>31</v>
       </c>
       <c r="S23" s="23"/>
       <c r="T23" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.45</v>
       </c>
-      <c r="U23" s="42">
+      <c r="U23" s="40">
         <f>ROUND(playerHealth/(T23),2)</f>
         <v>17.78</v>
       </c>
@@ -2784,7 +2843,7 @@
         <f>D23*(E23-0.2)</f>
         <v>0.3</v>
       </c>
-      <c r="W23" s="42">
+      <c r="W23" s="40">
         <f>ROUND(playerHealth/(V23),2)</f>
         <v>26.67</v>
       </c>
@@ -2794,7 +2853,7 @@
       <c r="A24" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="68">
+      <c r="B24" s="66">
         <v>650</v>
       </c>
       <c r="C24" s="23">
@@ -2834,7 +2893,7 @@
         <f>D24*E24*H24</f>
         <v>15</v>
       </c>
-      <c r="O24" s="41">
+      <c r="O24" s="39">
         <f>ROUND(playerHealth/(D24*E24),1)</f>
         <v>16</v>
       </c>
@@ -2846,7 +2905,7 @@
         <f>ROUND(C24/G24,3)</f>
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="R24" s="34" t="s">
+      <c r="R24" s="33" t="s">
         <v>31</v>
       </c>
       <c r="S24" s="23"/>
@@ -2854,7 +2913,7 @@
         <f xml:space="preserve"> D24*E24*9/10</f>
         <v>0.45</v>
       </c>
-      <c r="U24" s="42">
+      <c r="U24" s="40">
         <f>ROUND(playerHealth/(T24),2)</f>
         <v>17.78</v>
       </c>
@@ -2862,7 +2921,7 @@
         <f>D24*(E24-0.2)</f>
         <v>0.3</v>
       </c>
-      <c r="W24" s="42">
+      <c r="W24" s="40">
         <f>ROUND(playerHealth/(V24),2)</f>
         <v>26.67</v>
       </c>
@@ -2870,7 +2929,7 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A25" s="22"/>
-      <c r="B25" s="68"/>
+      <c r="B25" s="66"/>
       <c r="C25" s="23"/>
       <c r="D25" s="28"/>
       <c r="E25" s="23"/>
@@ -2886,19 +2945,19 @@
       <c r="O25" s="23"/>
       <c r="P25" s="23"/>
       <c r="Q25" s="23"/>
-      <c r="R25" s="40"/>
+      <c r="R25" s="38"/>
       <c r="S25" s="23"/>
       <c r="T25" s="23"/>
-      <c r="U25" s="42"/>
+      <c r="U25" s="40"/>
       <c r="V25" s="23"/>
-      <c r="W25" s="42"/>
+      <c r="W25" s="40"/>
       <c r="X25" s="23"/>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="68"/>
+      <c r="B26" s="66"/>
       <c r="C26" s="23"/>
       <c r="D26" s="24"/>
       <c r="E26" s="23"/>
@@ -2914,19 +2973,19 @@
       <c r="O26" s="23"/>
       <c r="P26" s="23"/>
       <c r="Q26" s="23"/>
-      <c r="R26" s="40"/>
+      <c r="R26" s="38"/>
       <c r="S26" s="23"/>
       <c r="T26" s="23"/>
-      <c r="U26" s="42"/>
+      <c r="U26" s="40"/>
       <c r="V26" s="23"/>
-      <c r="W26" s="42"/>
+      <c r="W26" s="40"/>
       <c r="X26" s="23"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A27" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="68">
+      <c r="B27" s="66">
         <v>24</v>
       </c>
       <c r="C27" s="23">
@@ -2967,21 +3026,21 @@
       </c>
       <c r="P27" s="23"/>
       <c r="Q27" s="23"/>
-      <c r="R27" s="40"/>
+      <c r="R27" s="38"/>
       <c r="S27" s="23"/>
       <c r="T27" s="23">
-        <f t="shared" ref="T27:T29" si="5" xml:space="preserve"> D27*E27*9/10</f>
+        <f t="shared" ref="T27:T29" si="8" xml:space="preserve"> D27*E27*9/10</f>
         <v>0.18</v>
       </c>
-      <c r="U27" s="42">
+      <c r="U27" s="40">
         <f>ROUND(playerHealth/(T27),2)</f>
         <v>44.44</v>
       </c>
       <c r="V27" s="23">
-        <f t="shared" ref="V27:V28" si="6">D27*(E27-0.2)</f>
+        <f t="shared" ref="V27:V28" si="9">D27*(E27-0.2)</f>
         <v>0</v>
       </c>
-      <c r="W27" s="42"/>
+      <c r="W27" s="40"/>
       <c r="X27" s="23"/>
       <c r="Y27" t="s">
         <v>55</v>
@@ -2991,7 +3050,7 @@
       <c r="A28" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="68">
+      <c r="B28" s="66">
         <v>32</v>
       </c>
       <c r="C28" s="23">
@@ -3032,21 +3091,21 @@
       </c>
       <c r="P28" s="23"/>
       <c r="Q28" s="23"/>
-      <c r="R28" s="40"/>
+      <c r="R28" s="38"/>
       <c r="S28" s="23"/>
       <c r="T28" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.36</v>
       </c>
-      <c r="U28" s="42">
+      <c r="U28" s="40">
         <f>ROUND(playerHealth/(T28),2)</f>
         <v>22.22</v>
       </c>
       <c r="V28" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.2</v>
       </c>
-      <c r="W28" s="42">
+      <c r="W28" s="40">
         <f>ROUND(playerHealth/(V28),2)</f>
         <v>40</v>
       </c>
@@ -3056,7 +3115,7 @@
       <c r="A29" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="68">
+      <c r="B29" s="66">
         <v>48</v>
       </c>
       <c r="C29" s="23">
@@ -3083,7 +3142,7 @@
       <c r="J29" s="23"/>
       <c r="K29" s="23"/>
       <c r="L29" s="23">
-        <f t="shared" ref="L29" si="7">ROUND(D29*E29/F29*1000,3)</f>
+        <f t="shared" ref="L29" si="10">ROUND(D29*E29/F29*1000,3)</f>
         <v>2</v>
       </c>
       <c r="M29" s="23">
@@ -3097,13 +3156,13 @@
       </c>
       <c r="P29" s="23"/>
       <c r="Q29" s="23"/>
-      <c r="R29" s="40"/>
+      <c r="R29" s="38"/>
       <c r="S29" s="23"/>
       <c r="T29" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.9</v>
       </c>
-      <c r="U29" s="41">
+      <c r="U29" s="39">
         <f>ROUND(playerHealth/(T29),2)</f>
         <v>8.89</v>
       </c>
@@ -3111,24 +3170,24 @@
         <f>D29*(E29-0.4)</f>
         <v>0.6</v>
       </c>
-      <c r="W29" s="41">
+      <c r="W29" s="39">
         <f>ROUND(playerHealth/(V29),2)</f>
         <v>13.33</v>
       </c>
       <c r="X29" s="23"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A30" s="44"/>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A31" s="46" t="s">
+      <c r="A31" s="44" t="s">
         <v>58</v>
       </c>
       <c r="B31" s="9" t="s">
@@ -3149,53 +3208,53 @@
       <c r="M31" s="9"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A32" s="47" t="s">
+      <c r="A32" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="48" t="s">
+      <c r="B32" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="45"/>
-      <c r="D32" s="48" t="s">
+      <c r="C32" s="43"/>
+      <c r="D32" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="E32" s="49"/>
-      <c r="F32" s="49" t="s">
+      <c r="E32" s="47"/>
+      <c r="F32" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="G32" s="49"/>
-      <c r="H32" s="49"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="50"/>
-      <c r="K32" s="50"/>
-      <c r="L32" s="50"/>
-      <c r="M32" s="50"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="48"/>
+      <c r="L32" s="48"/>
+      <c r="M32" s="48"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="48" t="s">
+      <c r="B33" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="45"/>
-      <c r="D33" s="48" t="s">
+      <c r="C33" s="43"/>
+      <c r="D33" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49" t="s">
+      <c r="E33" s="47"/>
+      <c r="F33" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="50"/>
-      <c r="K33" s="50"/>
-      <c r="L33" s="50"/>
-      <c r="M33" s="50"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="48"/>
+      <c r="K33" s="48"/>
+      <c r="L33" s="48"/>
+      <c r="M33" s="48"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A34" s="51"/>
+      <c r="A34" s="49"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
@@ -3219,171 +3278,171 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="F40" s="55" t="s">
+      <c r="F40" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="G40" s="55"/>
-      <c r="H40" s="55"/>
-      <c r="I40" s="55"/>
-      <c r="J40" s="55"/>
-      <c r="K40" s="55"/>
-      <c r="L40" s="55"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="53"/>
+      <c r="K40" s="53"/>
+      <c r="L40" s="53"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B41" s="76" t="s">
+      <c r="B41" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="G41" s="75" t="s">
+      <c r="G41" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="H41" s="75"/>
-      <c r="I41" s="75"/>
-      <c r="J41" s="75"/>
-      <c r="K41" s="75"/>
-      <c r="L41" s="75"/>
+      <c r="H41" s="73"/>
+      <c r="I41" s="73"/>
+      <c r="J41" s="73"/>
+      <c r="K41" s="73"/>
+      <c r="L41" s="73"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A42" s="52" t="s">
+      <c r="A42" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="B42" s="53">
+      <c r="B42" s="51">
         <v>-1</v>
       </c>
-      <c r="C42" s="53">
+      <c r="C42" s="51">
         <v>0</v>
       </c>
-      <c r="D42" s="53">
-        <v>1</v>
-      </c>
-      <c r="E42" s="53">
+      <c r="D42" s="51">
+        <v>1</v>
+      </c>
+      <c r="E42" s="51">
         <v>2</v>
       </c>
-      <c r="F42" s="56">
+      <c r="F42" s="54">
         <v>3</v>
       </c>
-      <c r="G42" s="56">
+      <c r="G42" s="54">
         <v>4</v>
       </c>
-      <c r="H42" s="56">
+      <c r="H42" s="54">
         <v>5</v>
       </c>
-      <c r="I42" s="56">
+      <c r="I42" s="54">
         <v>6</v>
       </c>
-      <c r="J42" s="56">
+      <c r="J42" s="54">
         <v>7</v>
       </c>
-      <c r="K42" s="56">
+      <c r="K42" s="54">
         <v>8</v>
       </c>
-      <c r="L42" s="56">
+      <c r="L42" s="54">
         <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A43" s="54" t="s">
+      <c r="A43" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="45">
-        <f>(2+B42)*tilesize</f>
+      <c r="B43" s="43">
+        <f t="shared" ref="B43:L43" si="11">(2+B42)*tilesize</f>
         <v>128</v>
       </c>
-      <c r="C43" s="45">
-        <f>(2+C42)*tilesize</f>
+      <c r="C43" s="43">
+        <f t="shared" si="11"/>
         <v>256</v>
       </c>
-      <c r="D43" s="45">
-        <f>(2+D42)*tilesize</f>
+      <c r="D43" s="43">
+        <f t="shared" si="11"/>
         <v>384</v>
       </c>
-      <c r="E43" s="45">
-        <f>(2+E42)*tilesize</f>
+      <c r="E43" s="43">
+        <f t="shared" si="11"/>
         <v>512</v>
       </c>
-      <c r="F43" s="45">
-        <f>(2+F42)*tilesize</f>
+      <c r="F43" s="43">
+        <f t="shared" si="11"/>
         <v>640</v>
       </c>
-      <c r="G43" s="45">
-        <f>(2+G42)*tilesize</f>
+      <c r="G43" s="43">
+        <f t="shared" si="11"/>
         <v>768</v>
       </c>
-      <c r="H43" s="45">
-        <f>(2+H42)*tilesize</f>
+      <c r="H43" s="43">
+        <f t="shared" si="11"/>
         <v>896</v>
       </c>
-      <c r="I43" s="45">
-        <f>(2+I42)*tilesize</f>
+      <c r="I43" s="43">
+        <f t="shared" si="11"/>
         <v>1024</v>
       </c>
-      <c r="J43" s="45">
-        <f>(2+J42)*tilesize</f>
+      <c r="J43" s="43">
+        <f t="shared" si="11"/>
         <v>1152</v>
       </c>
-      <c r="K43" s="45">
-        <f>(2+K42)*tilesize</f>
+      <c r="K43" s="43">
+        <f t="shared" si="11"/>
         <v>1280</v>
       </c>
-      <c r="L43" s="45">
-        <f>(2+L42)*tilesize</f>
+      <c r="L43" s="43">
+        <f t="shared" si="11"/>
         <v>1408</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A44" s="54" t="s">
+      <c r="A44" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="B44" s="57">
-        <f t="shared" ref="B44:L44" si="8">(2+B42+1)*tilesize+tilesize/2</f>
+      <c r="B44" s="55">
+        <f t="shared" ref="B44:L44" si="12">(2+B42+1)*tilesize+tilesize/2</f>
         <v>320</v>
       </c>
-      <c r="C44" s="58">
-        <f t="shared" si="8"/>
+      <c r="C44" s="56">
+        <f t="shared" si="12"/>
         <v>448</v>
       </c>
-      <c r="D44" s="59">
-        <f t="shared" si="8"/>
+      <c r="D44" s="57">
+        <f t="shared" si="12"/>
         <v>576</v>
       </c>
-      <c r="E44" s="60">
-        <f t="shared" si="8"/>
+      <c r="E44" s="58">
+        <f t="shared" si="12"/>
         <v>704</v>
       </c>
-      <c r="F44" s="61">
-        <f t="shared" si="8"/>
+      <c r="F44" s="59">
+        <f t="shared" si="12"/>
         <v>832</v>
       </c>
-      <c r="G44" s="62">
-        <f t="shared" si="8"/>
+      <c r="G44" s="60">
+        <f t="shared" si="12"/>
         <v>960</v>
       </c>
-      <c r="H44" s="63">
-        <f t="shared" si="8"/>
+      <c r="H44" s="61">
+        <f t="shared" si="12"/>
         <v>1088</v>
       </c>
-      <c r="I44" s="64">
-        <f t="shared" si="8"/>
+      <c r="I44" s="62">
+        <f t="shared" si="12"/>
         <v>1216</v>
       </c>
-      <c r="J44" s="65">
-        <f t="shared" si="8"/>
+      <c r="J44" s="63">
+        <f t="shared" si="12"/>
         <v>1344</v>
       </c>
-      <c r="K44" s="66">
-        <f t="shared" si="8"/>
+      <c r="K44" s="64">
+        <f t="shared" si="12"/>
         <v>1472</v>
       </c>
-      <c r="L44" s="67">
-        <f t="shared" si="8"/>
+      <c r="L44" s="65">
+        <f t="shared" si="12"/>
         <v>1600</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="C45" s="73" t="s">
+      <c r="C45" s="71" t="s">
         <v>84</v>
       </c>
-      <c r="D45" s="74"/>
-      <c r="E45" s="72"/>
+      <c r="D45" s="72"/>
+      <c r="E45" s="70"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
New explosion: shockwave Tankbuster and mine uses this explosion
</commit_message>
<xml_diff>
--- a/gun infos.xlsx
+++ b/gun infos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F81B20-76D3-433C-9FC2-C54FBD501EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAA2DAC-EE74-4C24-94B7-612B95AD999E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="0" windowWidth="33240" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,6 +24,7 @@
     <definedName name="health_cap">Sheet1!$N$61</definedName>
     <definedName name="player_radius">Sheet1!$B$60</definedName>
     <definedName name="playerHealth">Sheet1!$B$47</definedName>
+    <definedName name="shockWave_damage">Sheet1!$E$6</definedName>
     <definedName name="speed_cap">Sheet1!$P$61</definedName>
     <definedName name="tilesize">Sheet1!$B$48</definedName>
   </definedNames>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="136">
   <si>
     <t>Weapon info</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -600,6 +601,10 @@
   </si>
   <si>
     <t>Has a powerful machine gun attached to it</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shockWave</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1321,6 +1326,9 @@
     <xf numFmtId="0" fontId="28" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1331,9 +1339,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1618,8 +1623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P53" sqref="P53"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1915,7 +1920,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="28">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F5" s="28">
         <v>4000</v>
@@ -1933,22 +1938,22 @@
         <v>87</v>
       </c>
       <c r="K5" s="28">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="L5" s="23">
-        <f>ROUND(D5*(E5+fraghitnum2*frag_damage)/F5*1000,2)</f>
-        <v>31</v>
+        <f>ROUND(D5*(E5+fraghitnum2*shockWave_damage)/F5*1000,2)</f>
+        <v>35</v>
       </c>
       <c r="M5" s="23">
-        <f>ROUND(D5*(E5+fraghitnum2*frag_damage)/(F5+I5)*1000,2)</f>
-        <v>12.4</v>
+        <f>ROUND(D5*(E5+fraghitnum2*shockWave_damage)/(F5+I5)*1000,2)</f>
+        <v>14</v>
       </c>
       <c r="N5" s="23">
-        <f>D5*(E5+fraghitnum2*frag_damage)*H5</f>
-        <v>124</v>
+        <f>D5*(E5+fraghitnum2*shockWave_damage)*H5</f>
+        <v>140</v>
       </c>
       <c r="O5" s="29">
-        <f>ROUND(playerHealth/(D5*(E5+fraghitnum2*frag_damage)),1)</f>
+        <f>ROUND(playerHealth/(D5*(E5+fraghitnum2*shockWave_damage)),1)</f>
         <v>0.1</v>
       </c>
       <c r="P5" s="23">
@@ -1964,16 +1969,16 @@
       </c>
       <c r="S5" s="23"/>
       <c r="T5" s="23">
-        <f xml:space="preserve"> D5*E5*7/10 +D5*fraghitnum2*frag_damage*9/10</f>
-        <v>91.6</v>
+        <f xml:space="preserve"> D5*E5*7/10 +D5*fraghitnum2*shockWave_damage*7/10</f>
+        <v>98</v>
       </c>
       <c r="U5" s="32">
         <f>ROUND(playerHealth/(T5),2)</f>
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="V5" s="23">
-        <f>D5*((E5+fraghitnum2*frag_damage)-0.4)</f>
-        <v>123.6</v>
+        <f>D5*((E5+fraghitnum2*shockWave_damage)-0.4)</f>
+        <v>139.6</v>
       </c>
       <c r="W5" s="32">
         <f>ROUND(playerHealth/(V5),2)</f>
@@ -1985,11 +1990,15 @@
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A6" s="27"/>
+      <c r="A6" s="27" t="s">
+        <v>135</v>
+      </c>
       <c r="B6" s="82"/>
       <c r="C6" s="72"/>
       <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
+      <c r="E6" s="72">
+        <v>15</v>
+      </c>
       <c r="F6" s="72"/>
       <c r="G6" s="72"/>
       <c r="H6" s="72"/>
@@ -4000,10 +4009,10 @@
       <c r="R60" t="s">
         <v>123</v>
       </c>
-      <c r="AF60" s="99"/>
-      <c r="AG60" s="99"/>
-      <c r="AH60" s="99"/>
-      <c r="AI60" s="99"/>
+      <c r="AF60" s="100"/>
+      <c r="AG60" s="100"/>
+      <c r="AH60" s="100"/>
+      <c r="AI60" s="100"/>
     </row>
     <row r="61" spans="1:35" x14ac:dyDescent="0.45">
       <c r="N61">
@@ -4021,19 +4030,19 @@
       <c r="R61">
         <v>10</v>
       </c>
-      <c r="AF61" s="100"/>
-      <c r="AG61" s="100"/>
-      <c r="AH61" s="100"/>
-      <c r="AI61" s="100"/>
+      <c r="AF61" s="101"/>
+      <c r="AG61" s="101"/>
+      <c r="AH61" s="101"/>
+      <c r="AI61" s="101"/>
     </row>
     <row r="62" spans="1:35" x14ac:dyDescent="0.45">
       <c r="H62" t="s">
         <v>105</v>
       </c>
-      <c r="I62" s="98" t="s">
+      <c r="I62" s="99" t="s">
         <v>109</v>
       </c>
-      <c r="J62" s="98"/>
+      <c r="J62" s="99"/>
       <c r="K62" t="s">
         <v>110</v>
       </c>
@@ -4041,17 +4050,17 @@
         <f>COUNTIF(G3:G35,"&gt;0")</f>
         <v>21</v>
       </c>
-      <c r="N62" s="97" t="s">
+      <c r="N62" s="98" t="s">
         <v>115</v>
       </c>
-      <c r="O62" s="97"/>
-      <c r="P62" s="97"/>
-      <c r="Q62" s="97"/>
-      <c r="R62" s="97"/>
-      <c r="AF62" s="100"/>
-      <c r="AG62" s="100"/>
-      <c r="AH62" s="100"/>
-      <c r="AI62" s="100"/>
+      <c r="O62" s="98"/>
+      <c r="P62" s="98"/>
+      <c r="Q62" s="98"/>
+      <c r="R62" s="98"/>
+      <c r="AF62" s="101"/>
+      <c r="AG62" s="101"/>
+      <c r="AH62" s="101"/>
+      <c r="AI62" s="101"/>
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A63" s="48" t="s">
@@ -4101,20 +4110,20 @@
         <v>122</v>
       </c>
       <c r="S63" s="49"/>
-      <c r="T63" s="99" t="s">
+      <c r="T63" s="100" t="s">
         <v>126</v>
       </c>
-      <c r="U63" s="99"/>
+      <c r="U63" s="100"/>
       <c r="V63" s="49" t="s">
         <v>24</v>
       </c>
       <c r="W63" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="AF63" s="100"/>
-      <c r="AG63" s="100"/>
-      <c r="AH63" s="100"/>
-      <c r="AI63" s="100"/>
+      <c r="AF63" s="101"/>
+      <c r="AG63" s="101"/>
+      <c r="AH63" s="101"/>
+      <c r="AI63" s="101"/>
     </row>
     <row r="64" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A64" s="22" t="s">
@@ -4172,21 +4181,21 @@
         <v>10.5</v>
       </c>
       <c r="S64" s="86"/>
-      <c r="T64" s="101">
+      <c r="T64" s="97">
         <f>Q64+N64+O64</f>
         <v>4.5</v>
       </c>
-      <c r="U64" s="101"/>
+      <c r="U64" s="97"/>
       <c r="V64" s="33" t="s">
         <v>31</v>
       </c>
       <c r="W64" t="s">
         <v>133</v>
       </c>
-      <c r="AF64" s="100"/>
-      <c r="AG64" s="100"/>
-      <c r="AH64" s="100"/>
-      <c r="AI64" s="100"/>
+      <c r="AF64" s="101"/>
+      <c r="AG64" s="101"/>
+      <c r="AH64" s="101"/>
+      <c r="AI64" s="101"/>
     </row>
     <row r="65" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A65" s="22" t="s">
@@ -4244,21 +4253,21 @@
         <v>12.3</v>
       </c>
       <c r="S65" s="86"/>
-      <c r="T65" s="101">
+      <c r="T65" s="97">
         <f t="shared" ref="T65:T70" si="17">Q65+N65+O65</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="U65" s="101"/>
+      <c r="U65" s="97"/>
       <c r="V65" s="33" t="s">
         <v>31</v>
       </c>
       <c r="W65" t="s">
         <v>132</v>
       </c>
-      <c r="AF65" s="100"/>
-      <c r="AG65" s="100"/>
-      <c r="AH65" s="100"/>
-      <c r="AI65" s="100"/>
+      <c r="AF65" s="101"/>
+      <c r="AG65" s="101"/>
+      <c r="AH65" s="101"/>
+      <c r="AI65" s="101"/>
     </row>
     <row r="66" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A66" s="22" t="s">
@@ -4316,21 +4325,21 @@
         <v>14.399999999999999</v>
       </c>
       <c r="S66" s="86"/>
-      <c r="T66" s="101">
+      <c r="T66" s="97">
         <f t="shared" si="17"/>
         <v>10.399999999999999</v>
       </c>
-      <c r="U66" s="101"/>
+      <c r="U66" s="97"/>
       <c r="V66" s="33" t="s">
         <v>31</v>
       </c>
       <c r="W66" t="s">
         <v>134</v>
       </c>
-      <c r="AF66" s="100"/>
-      <c r="AG66" s="100"/>
-      <c r="AH66" s="100"/>
-      <c r="AI66" s="100"/>
+      <c r="AF66" s="101"/>
+      <c r="AG66" s="101"/>
+      <c r="AH66" s="101"/>
+      <c r="AI66" s="101"/>
     </row>
     <row r="67" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A67" s="22" t="s">
@@ -4388,11 +4397,11 @@
         <v>18.700000000000003</v>
       </c>
       <c r="S67" s="86"/>
-      <c r="T67" s="101">
+      <c r="T67" s="97">
         <f t="shared" si="17"/>
         <v>17.7</v>
       </c>
-      <c r="U67" s="101"/>
+      <c r="U67" s="97"/>
       <c r="V67" s="26" t="s">
         <v>30</v>
       </c>
@@ -4456,11 +4465,11 @@
         <v>17.100000000000001</v>
       </c>
       <c r="S68" s="86"/>
-      <c r="T68" s="101">
+      <c r="T68" s="97">
         <f t="shared" si="17"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="U68" s="101"/>
+      <c r="U68" s="97"/>
       <c r="V68" s="33" t="s">
         <v>31</v>
       </c>
@@ -4524,11 +4533,11 @@
         <v>18.8</v>
       </c>
       <c r="S69" s="86"/>
-      <c r="T69" s="101">
+      <c r="T69" s="97">
         <f t="shared" si="17"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="U69" s="101"/>
+      <c r="U69" s="97"/>
       <c r="V69" s="26" t="s">
         <v>30</v>
       </c>
@@ -4592,11 +4601,11 @@
         <v>25.799999999999997</v>
       </c>
       <c r="S70" s="86"/>
-      <c r="T70" s="101">
+      <c r="T70" s="97">
         <f t="shared" si="17"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="U70" s="101"/>
+      <c r="U70" s="97"/>
       <c r="V70" s="30" t="s">
         <v>80</v>
       </c>
@@ -4606,11 +4615,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="T67:U67"/>
-    <mergeCell ref="T68:U68"/>
-    <mergeCell ref="T66:U66"/>
-    <mergeCell ref="T69:U69"/>
-    <mergeCell ref="T70:U70"/>
     <mergeCell ref="N62:R62"/>
     <mergeCell ref="I62:J62"/>
     <mergeCell ref="AF60:AI60"/>
@@ -4623,6 +4627,11 @@
     <mergeCell ref="T63:U63"/>
     <mergeCell ref="T64:U64"/>
     <mergeCell ref="T65:U65"/>
+    <mergeCell ref="T67:U67"/>
+    <mergeCell ref="T68:U68"/>
+    <mergeCell ref="T66:U66"/>
+    <mergeCell ref="T69:U69"/>
+    <mergeCell ref="T70:U70"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Plane design: more transparent
</commit_message>
<xml_diff>
--- a/gun infos.xlsx
+++ b/gun infos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1521A332-F3F7-4AB7-B407-D15EFACF9ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECE408A-E0C2-4A8C-AF31-AA341BB6F235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="159">
   <si>
     <t>Weapon info</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -645,6 +645,57 @@
   </si>
   <si>
     <t>total damage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Airstrike</t>
+  </si>
+  <si>
+    <t>Color</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>red</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>green</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yellow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>white</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrikeNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOMB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SUPPLY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQUEST VEHICLE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRANSPORT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 ~ 5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1374,6 +1425,18 @@
     <xf numFmtId="0" fontId="28" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1381,18 +1444,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1675,10 +1726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI76"/>
+  <dimension ref="A1:AI86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H79" sqref="H79"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA55" sqref="AA55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -4115,10 +4166,10 @@
       <c r="R60" t="s">
         <v>122</v>
       </c>
-      <c r="AF60" s="99"/>
-      <c r="AG60" s="99"/>
-      <c r="AH60" s="99"/>
-      <c r="AI60" s="99"/>
+      <c r="AF60" s="103"/>
+      <c r="AG60" s="103"/>
+      <c r="AH60" s="103"/>
+      <c r="AI60" s="103"/>
     </row>
     <row r="61" spans="1:35" x14ac:dyDescent="0.45">
       <c r="N61">
@@ -4136,19 +4187,19 @@
       <c r="R61">
         <v>10</v>
       </c>
-      <c r="AF61" s="100"/>
-      <c r="AG61" s="100"/>
-      <c r="AH61" s="100"/>
-      <c r="AI61" s="100"/>
+      <c r="AF61" s="99"/>
+      <c r="AG61" s="99"/>
+      <c r="AH61" s="99"/>
+      <c r="AI61" s="99"/>
     </row>
     <row r="62" spans="1:35" x14ac:dyDescent="0.45">
       <c r="H62" t="s">
         <v>104</v>
       </c>
-      <c r="I62" s="98" t="s">
+      <c r="I62" s="102" t="s">
         <v>108</v>
       </c>
-      <c r="J62" s="98"/>
+      <c r="J62" s="102"/>
       <c r="K62" t="s">
         <v>109</v>
       </c>
@@ -4156,17 +4207,17 @@
         <f>COUNTIF(G3:G35,"&gt;0")</f>
         <v>22</v>
       </c>
-      <c r="N62" s="97" t="s">
+      <c r="N62" s="101" t="s">
         <v>114</v>
       </c>
-      <c r="O62" s="97"/>
-      <c r="P62" s="97"/>
-      <c r="Q62" s="97"/>
-      <c r="R62" s="97"/>
-      <c r="AF62" s="100"/>
-      <c r="AG62" s="100"/>
-      <c r="AH62" s="100"/>
-      <c r="AI62" s="100"/>
+      <c r="O62" s="101"/>
+      <c r="P62" s="101"/>
+      <c r="Q62" s="101"/>
+      <c r="R62" s="101"/>
+      <c r="AF62" s="99"/>
+      <c r="AG62" s="99"/>
+      <c r="AH62" s="99"/>
+      <c r="AI62" s="99"/>
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A63" s="48" t="s">
@@ -4216,20 +4267,20 @@
         <v>121</v>
       </c>
       <c r="S63" s="49"/>
-      <c r="T63" s="99" t="s">
+      <c r="T63" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="U63" s="99"/>
+      <c r="U63" s="103"/>
       <c r="V63" s="49" t="s">
         <v>24</v>
       </c>
       <c r="W63" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="AF63" s="100"/>
-      <c r="AG63" s="100"/>
-      <c r="AH63" s="100"/>
-      <c r="AI63" s="100"/>
+      <c r="AF63" s="99"/>
+      <c r="AG63" s="99"/>
+      <c r="AH63" s="99"/>
+      <c r="AI63" s="99"/>
     </row>
     <row r="64" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A64" s="22" t="s">
@@ -4287,21 +4338,21 @@
         <v>10.100000000000001</v>
       </c>
       <c r="S64" s="86"/>
-      <c r="T64" s="101">
+      <c r="T64" s="100">
         <f>Q64+N64+O64</f>
         <v>4.1000000000000005</v>
       </c>
-      <c r="U64" s="101"/>
+      <c r="U64" s="100"/>
       <c r="V64" s="33" t="s">
         <v>31</v>
       </c>
       <c r="W64" t="s">
         <v>132</v>
       </c>
-      <c r="AF64" s="100"/>
-      <c r="AG64" s="100"/>
-      <c r="AH64" s="100"/>
-      <c r="AI64" s="100"/>
+      <c r="AF64" s="99"/>
+      <c r="AG64" s="99"/>
+      <c r="AH64" s="99"/>
+      <c r="AI64" s="99"/>
     </row>
     <row r="65" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A65" s="22" t="s">
@@ -4359,21 +4410,21 @@
         <v>12.3</v>
       </c>
       <c r="S65" s="86"/>
-      <c r="T65" s="101">
+      <c r="T65" s="100">
         <f t="shared" ref="T65:T70" si="21">Q65+N65+O65</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="U65" s="101"/>
+      <c r="U65" s="100"/>
       <c r="V65" s="33" t="s">
         <v>31</v>
       </c>
       <c r="W65" t="s">
         <v>131</v>
       </c>
-      <c r="AF65" s="100"/>
-      <c r="AG65" s="100"/>
-      <c r="AH65" s="100"/>
-      <c r="AI65" s="100"/>
+      <c r="AF65" s="99"/>
+      <c r="AG65" s="99"/>
+      <c r="AH65" s="99"/>
+      <c r="AI65" s="99"/>
     </row>
     <row r="66" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A66" s="22" t="s">
@@ -4431,21 +4482,21 @@
         <v>14.399999999999999</v>
       </c>
       <c r="S66" s="86"/>
-      <c r="T66" s="101">
+      <c r="T66" s="100">
         <f t="shared" si="21"/>
         <v>10.399999999999999</v>
       </c>
-      <c r="U66" s="101"/>
+      <c r="U66" s="100"/>
       <c r="V66" s="33" t="s">
         <v>31</v>
       </c>
       <c r="W66" t="s">
         <v>133</v>
       </c>
-      <c r="AF66" s="100"/>
-      <c r="AG66" s="100"/>
-      <c r="AH66" s="100"/>
-      <c r="AI66" s="100"/>
+      <c r="AF66" s="99"/>
+      <c r="AG66" s="99"/>
+      <c r="AH66" s="99"/>
+      <c r="AI66" s="99"/>
     </row>
     <row r="67" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A67" s="22" t="s">
@@ -4503,11 +4554,11 @@
         <v>18.700000000000003</v>
       </c>
       <c r="S67" s="86"/>
-      <c r="T67" s="101">
+      <c r="T67" s="100">
         <f t="shared" si="21"/>
         <v>17.7</v>
       </c>
-      <c r="U67" s="101"/>
+      <c r="U67" s="100"/>
       <c r="V67" s="26" t="s">
         <v>30</v>
       </c>
@@ -4571,11 +4622,11 @@
         <v>17.100000000000001</v>
       </c>
       <c r="S68" s="86"/>
-      <c r="T68" s="101">
+      <c r="T68" s="100">
         <f t="shared" si="21"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="U68" s="101"/>
+      <c r="U68" s="100"/>
       <c r="V68" s="33" t="s">
         <v>31</v>
       </c>
@@ -4639,11 +4690,11 @@
         <v>18.8</v>
       </c>
       <c r="S69" s="86"/>
-      <c r="T69" s="101">
+      <c r="T69" s="100">
         <f t="shared" si="21"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="U69" s="101"/>
+      <c r="U69" s="100"/>
       <c r="V69" s="26" t="s">
         <v>30</v>
       </c>
@@ -4707,11 +4758,11 @@
         <v>25.799999999999997</v>
       </c>
       <c r="S70" s="86"/>
-      <c r="T70" s="101">
+      <c r="T70" s="100">
         <f t="shared" si="21"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="U70" s="101"/>
+      <c r="U70" s="100"/>
       <c r="V70" s="30" t="s">
         <v>79</v>
       </c>
@@ -4723,31 +4774,31 @@
       <c r="A74" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="B74" s="102" t="s">
+      <c r="B74" s="97" t="s">
         <v>98</v>
       </c>
-      <c r="C74" s="102" t="s">
+      <c r="C74" s="97" t="s">
         <v>97</v>
       </c>
-      <c r="D74" s="102" t="s">
+      <c r="D74" s="97" t="s">
         <v>143</v>
       </c>
-      <c r="E74" s="103" t="s">
+      <c r="E74" s="98" t="s">
         <v>144</v>
       </c>
-      <c r="F74" s="103"/>
-      <c r="G74" s="103" t="s">
+      <c r="F74" s="98"/>
+      <c r="G74" s="98" t="s">
         <v>145</v>
       </c>
-      <c r="H74" s="103"/>
-      <c r="I74" s="102"/>
-      <c r="J74" s="102"/>
-      <c r="K74" s="103" t="s">
+      <c r="H74" s="98"/>
+      <c r="I74" s="97"/>
+      <c r="J74" s="97"/>
+      <c r="K74" s="98" t="s">
         <v>142</v>
       </c>
-      <c r="L74" s="103"/>
-      <c r="M74" s="103"/>
-      <c r="N74" s="103"/>
+      <c r="L74" s="98"/>
+      <c r="M74" s="98"/>
+      <c r="N74" s="98"/>
     </row>
     <row r="75" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A75" s="44" t="s">
@@ -4762,23 +4813,23 @@
       <c r="D75" s="86">
         <v>18</v>
       </c>
-      <c r="E75" s="100" t="s">
+      <c r="E75" s="99" t="s">
         <v>70</v>
       </c>
-      <c r="F75" s="100"/>
-      <c r="G75" s="100">
+      <c r="F75" s="99"/>
+      <c r="G75" s="99">
         <f>D75*frag_damage</f>
         <v>36</v>
       </c>
-      <c r="H75" s="100"/>
+      <c r="H75" s="99"/>
       <c r="I75" s="86"/>
       <c r="J75" s="86"/>
-      <c r="K75" s="100" t="s">
+      <c r="K75" s="99" t="s">
         <v>141</v>
       </c>
-      <c r="L75" s="100"/>
-      <c r="M75" s="100"/>
-      <c r="N75" s="100"/>
+      <c r="L75" s="99"/>
+      <c r="M75" s="99"/>
+      <c r="N75" s="99"/>
     </row>
     <row r="76" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A76" s="44" t="s">
@@ -4793,40 +4844,145 @@
       <c r="D76" s="86">
         <v>12</v>
       </c>
-      <c r="E76" s="100" t="s">
+      <c r="E76" s="99" t="s">
         <v>134</v>
       </c>
-      <c r="F76" s="100"/>
-      <c r="G76" s="100">
+      <c r="F76" s="99"/>
+      <c r="G76" s="99">
         <f>D76*shockWave_damage</f>
         <v>180</v>
       </c>
-      <c r="H76" s="100"/>
+      <c r="H76" s="99"/>
       <c r="I76" s="86"/>
       <c r="J76" s="86"/>
-      <c r="K76" s="100" t="s">
+      <c r="K76" s="99" t="s">
         <v>140</v>
       </c>
-      <c r="L76" s="100"/>
-      <c r="M76" s="100"/>
-      <c r="N76" s="100"/>
+      <c r="L76" s="99"/>
+      <c r="M76" s="99"/>
+      <c r="N76" s="99"/>
+    </row>
+    <row r="80" spans="1:35" x14ac:dyDescent="0.45">
+      <c r="A80" s="43" t="s">
+        <v>146</v>
+      </c>
+      <c r="B80" s="97" t="s">
+        <v>147</v>
+      </c>
+      <c r="C80" s="97" t="s">
+        <v>99</v>
+      </c>
+      <c r="D80" s="97" t="s">
+        <v>153</v>
+      </c>
+      <c r="E80" s="98" t="s">
+        <v>148</v>
+      </c>
+      <c r="F80" s="98"/>
+      <c r="G80" s="98"/>
+      <c r="H80" s="98"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A81" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="B81" s="83" t="s">
+        <v>149</v>
+      </c>
+      <c r="C81" s="41">
+        <v>12</v>
+      </c>
+      <c r="D81" s="85">
+        <v>16</v>
+      </c>
+      <c r="E81" s="99"/>
+      <c r="F81" s="99"/>
+      <c r="G81" s="99"/>
+      <c r="H81" s="99"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A82" s="44" t="s">
+        <v>155</v>
+      </c>
+      <c r="B82" s="83" t="s">
+        <v>150</v>
+      </c>
+      <c r="C82" s="85" t="s">
+        <v>158</v>
+      </c>
+      <c r="D82" s="85">
+        <v>1</v>
+      </c>
+      <c r="E82" s="99"/>
+      <c r="F82" s="99"/>
+      <c r="G82" s="99"/>
+      <c r="H82" s="99"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A83" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="B83" s="83" t="s">
+        <v>151</v>
+      </c>
+      <c r="C83" s="85" t="s">
+        <v>158</v>
+      </c>
+      <c r="D83" s="85">
+        <v>1</v>
+      </c>
+      <c r="E83" s="99"/>
+      <c r="F83" s="99"/>
+      <c r="G83" s="99"/>
+      <c r="H83" s="99"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A84" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="B84" s="83" t="s">
+        <v>152</v>
+      </c>
+      <c r="C84" s="85">
+        <v>6</v>
+      </c>
+      <c r="D84" s="85">
+        <v>1</v>
+      </c>
+      <c r="E84" s="99"/>
+      <c r="F84" s="99"/>
+      <c r="G84" s="99"/>
+      <c r="H84" s="99"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A85" s="44"/>
+      <c r="B85" s="83"/>
+      <c r="C85" s="86"/>
+      <c r="D85" s="86"/>
+      <c r="E85" s="99"/>
+      <c r="F85" s="99"/>
+      <c r="G85" s="99"/>
+      <c r="H85" s="99"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A86" s="44"/>
+      <c r="B86" s="83"/>
+      <c r="C86" s="86"/>
+      <c r="D86" s="86"/>
+      <c r="E86" s="99"/>
+      <c r="F86" s="99"/>
+      <c r="G86" s="99"/>
+      <c r="H86" s="99"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="K74:N74"/>
-    <mergeCell ref="K75:N75"/>
-    <mergeCell ref="K76:N76"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="E76:F76"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="G75:H75"/>
-    <mergeCell ref="G76:H76"/>
-    <mergeCell ref="T67:U67"/>
-    <mergeCell ref="T68:U68"/>
-    <mergeCell ref="T66:U66"/>
-    <mergeCell ref="T69:U69"/>
-    <mergeCell ref="T70:U70"/>
+  <mergeCells count="33">
+    <mergeCell ref="E85:H85"/>
+    <mergeCell ref="E86:H86"/>
+    <mergeCell ref="E80:H80"/>
+    <mergeCell ref="E81:H81"/>
+    <mergeCell ref="E82:H82"/>
+    <mergeCell ref="E83:H83"/>
+    <mergeCell ref="E84:H84"/>
     <mergeCell ref="N62:R62"/>
     <mergeCell ref="I62:J62"/>
     <mergeCell ref="AF60:AI60"/>
@@ -4839,6 +4995,20 @@
     <mergeCell ref="T63:U63"/>
     <mergeCell ref="T64:U64"/>
     <mergeCell ref="T65:U65"/>
+    <mergeCell ref="T67:U67"/>
+    <mergeCell ref="T68:U68"/>
+    <mergeCell ref="T66:U66"/>
+    <mergeCell ref="T69:U69"/>
+    <mergeCell ref="T70:U70"/>
+    <mergeCell ref="K74:N74"/>
+    <mergeCell ref="K75:N75"/>
+    <mergeCell ref="K76:N76"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="G76:H76"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
balance patch: slower speed of tank buster
</commit_message>
<xml_diff>
--- a/gun infos.xlsx
+++ b/gun infos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B551001C-533D-479D-A8C4-C799A9D1DE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE69AB61-FFCD-45A7-9C38-0C8544DD4AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1457,11 +1457,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1470,12 +1476,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1760,7 +1760,7 @@
   <dimension ref="A1:AI86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2063,7 +2063,7 @@
         <v>4000</v>
       </c>
       <c r="G5" s="28">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H5" s="28">
         <v>1</v>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="P5" s="23">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="23">
         <f t="shared" si="1"/>
@@ -4197,10 +4197,10 @@
       <c r="R60" t="s">
         <v>122</v>
       </c>
-      <c r="AF60" s="102"/>
-      <c r="AG60" s="102"/>
-      <c r="AH60" s="102"/>
-      <c r="AI60" s="102"/>
+      <c r="AF60" s="104"/>
+      <c r="AG60" s="104"/>
+      <c r="AH60" s="104"/>
+      <c r="AI60" s="104"/>
     </row>
     <row r="61" spans="1:35" x14ac:dyDescent="0.45">
       <c r="N61">
@@ -4218,19 +4218,19 @@
       <c r="R61">
         <v>10</v>
       </c>
-      <c r="AF61" s="98"/>
-      <c r="AG61" s="98"/>
-      <c r="AH61" s="98"/>
-      <c r="AI61" s="98"/>
+      <c r="AF61" s="100"/>
+      <c r="AG61" s="100"/>
+      <c r="AH61" s="100"/>
+      <c r="AI61" s="100"/>
     </row>
     <row r="62" spans="1:35" x14ac:dyDescent="0.45">
       <c r="H62" t="s">
         <v>104</v>
       </c>
-      <c r="I62" s="101" t="s">
+      <c r="I62" s="103" t="s">
         <v>108</v>
       </c>
-      <c r="J62" s="101"/>
+      <c r="J62" s="103"/>
       <c r="K62" t="s">
         <v>109</v>
       </c>
@@ -4238,17 +4238,17 @@
         <f>COUNTIF(G3:G35,"&gt;0")</f>
         <v>22</v>
       </c>
-      <c r="N62" s="100" t="s">
+      <c r="N62" s="102" t="s">
         <v>114</v>
       </c>
-      <c r="O62" s="100"/>
-      <c r="P62" s="100"/>
-      <c r="Q62" s="100"/>
-      <c r="R62" s="100"/>
-      <c r="AF62" s="98"/>
-      <c r="AG62" s="98"/>
-      <c r="AH62" s="98"/>
-      <c r="AI62" s="98"/>
+      <c r="O62" s="102"/>
+      <c r="P62" s="102"/>
+      <c r="Q62" s="102"/>
+      <c r="R62" s="102"/>
+      <c r="AF62" s="100"/>
+      <c r="AG62" s="100"/>
+      <c r="AH62" s="100"/>
+      <c r="AI62" s="100"/>
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A63" s="48" t="s">
@@ -4298,20 +4298,20 @@
         <v>121</v>
       </c>
       <c r="S63" s="49"/>
-      <c r="T63" s="102" t="s">
+      <c r="T63" s="104" t="s">
         <v>125</v>
       </c>
-      <c r="U63" s="102"/>
+      <c r="U63" s="104"/>
       <c r="V63" s="49" t="s">
         <v>24</v>
       </c>
       <c r="W63" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="AF63" s="98"/>
-      <c r="AG63" s="98"/>
-      <c r="AH63" s="98"/>
-      <c r="AI63" s="98"/>
+      <c r="AF63" s="100"/>
+      <c r="AG63" s="100"/>
+      <c r="AH63" s="100"/>
+      <c r="AI63" s="100"/>
     </row>
     <row r="64" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A64" s="22" t="s">
@@ -4369,21 +4369,21 @@
         <v>10.100000000000001</v>
       </c>
       <c r="S64" s="86"/>
-      <c r="T64" s="103">
+      <c r="T64" s="101">
         <f>Q64+N64+O64</f>
         <v>4.1000000000000005</v>
       </c>
-      <c r="U64" s="103"/>
+      <c r="U64" s="101"/>
       <c r="V64" s="33" t="s">
         <v>31</v>
       </c>
       <c r="W64" t="s">
         <v>132</v>
       </c>
-      <c r="AF64" s="98"/>
-      <c r="AG64" s="98"/>
-      <c r="AH64" s="98"/>
-      <c r="AI64" s="98"/>
+      <c r="AF64" s="100"/>
+      <c r="AG64" s="100"/>
+      <c r="AH64" s="100"/>
+      <c r="AI64" s="100"/>
     </row>
     <row r="65" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A65" s="22" t="s">
@@ -4441,21 +4441,21 @@
         <v>12.3</v>
       </c>
       <c r="S65" s="86"/>
-      <c r="T65" s="103">
+      <c r="T65" s="101">
         <f t="shared" ref="T65:T70" si="21">Q65+N65+O65</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="U65" s="103"/>
+      <c r="U65" s="101"/>
       <c r="V65" s="33" t="s">
         <v>31</v>
       </c>
       <c r="W65" t="s">
         <v>131</v>
       </c>
-      <c r="AF65" s="98"/>
-      <c r="AG65" s="98"/>
-      <c r="AH65" s="98"/>
-      <c r="AI65" s="98"/>
+      <c r="AF65" s="100"/>
+      <c r="AG65" s="100"/>
+      <c r="AH65" s="100"/>
+      <c r="AI65" s="100"/>
     </row>
     <row r="66" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A66" s="22" t="s">
@@ -4513,21 +4513,21 @@
         <v>14.399999999999999</v>
       </c>
       <c r="S66" s="86"/>
-      <c r="T66" s="103">
+      <c r="T66" s="101">
         <f t="shared" si="21"/>
         <v>10.399999999999999</v>
       </c>
-      <c r="U66" s="103"/>
+      <c r="U66" s="101"/>
       <c r="V66" s="33" t="s">
         <v>31</v>
       </c>
       <c r="W66" t="s">
         <v>133</v>
       </c>
-      <c r="AF66" s="98"/>
-      <c r="AG66" s="98"/>
-      <c r="AH66" s="98"/>
-      <c r="AI66" s="98"/>
+      <c r="AF66" s="100"/>
+      <c r="AG66" s="100"/>
+      <c r="AH66" s="100"/>
+      <c r="AI66" s="100"/>
     </row>
     <row r="67" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A67" s="22" t="s">
@@ -4585,11 +4585,11 @@
         <v>18.700000000000003</v>
       </c>
       <c r="S67" s="86"/>
-      <c r="T67" s="103">
+      <c r="T67" s="101">
         <f t="shared" si="21"/>
         <v>17.7</v>
       </c>
-      <c r="U67" s="103"/>
+      <c r="U67" s="101"/>
       <c r="V67" s="26" t="s">
         <v>30</v>
       </c>
@@ -4653,11 +4653,11 @@
         <v>17.100000000000001</v>
       </c>
       <c r="S68" s="86"/>
-      <c r="T68" s="103">
+      <c r="T68" s="101">
         <f t="shared" si="21"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="U68" s="103"/>
+      <c r="U68" s="101"/>
       <c r="V68" s="33" t="s">
         <v>31</v>
       </c>
@@ -4721,11 +4721,11 @@
         <v>18.8</v>
       </c>
       <c r="S69" s="86"/>
-      <c r="T69" s="103">
+      <c r="T69" s="101">
         <f t="shared" si="21"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="U69" s="103"/>
+      <c r="U69" s="101"/>
       <c r="V69" s="26" t="s">
         <v>30</v>
       </c>
@@ -4789,11 +4789,11 @@
         <v>25.799999999999997</v>
       </c>
       <c r="S70" s="86"/>
-      <c r="T70" s="103">
+      <c r="T70" s="101">
         <f t="shared" si="21"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="U70" s="103"/>
+      <c r="U70" s="101"/>
       <c r="V70" s="30" t="s">
         <v>79</v>
       </c>
@@ -4844,23 +4844,23 @@
       <c r="D75" s="86">
         <v>18</v>
       </c>
-      <c r="E75" s="98" t="s">
+      <c r="E75" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="F75" s="98"/>
-      <c r="G75" s="98">
+      <c r="F75" s="100"/>
+      <c r="G75" s="100">
         <f>D75*frag_damage</f>
         <v>36</v>
       </c>
-      <c r="H75" s="98"/>
+      <c r="H75" s="100"/>
       <c r="I75" s="86"/>
       <c r="J75" s="86"/>
-      <c r="K75" s="98" t="s">
+      <c r="K75" s="100" t="s">
         <v>141</v>
       </c>
-      <c r="L75" s="98"/>
-      <c r="M75" s="98"/>
-      <c r="N75" s="98"/>
+      <c r="L75" s="100"/>
+      <c r="M75" s="100"/>
+      <c r="N75" s="100"/>
     </row>
     <row r="76" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A76" s="44" t="s">
@@ -4875,23 +4875,23 @@
       <c r="D76" s="86">
         <v>12</v>
       </c>
-      <c r="E76" s="98" t="s">
+      <c r="E76" s="100" t="s">
         <v>134</v>
       </c>
-      <c r="F76" s="98"/>
-      <c r="G76" s="98">
+      <c r="F76" s="100"/>
+      <c r="G76" s="100">
         <f>D76*shockWave_damage</f>
         <v>180</v>
       </c>
-      <c r="H76" s="98"/>
+      <c r="H76" s="100"/>
       <c r="I76" s="86"/>
       <c r="J76" s="86"/>
-      <c r="K76" s="98" t="s">
+      <c r="K76" s="100" t="s">
         <v>140</v>
       </c>
-      <c r="L76" s="98"/>
-      <c r="M76" s="98"/>
-      <c r="N76" s="98"/>
+      <c r="L76" s="100"/>
+      <c r="M76" s="100"/>
+      <c r="N76" s="100"/>
     </row>
     <row r="80" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A80" s="43" t="s">
@@ -4946,32 +4946,32 @@
       <c r="D81" s="85">
         <v>16</v>
       </c>
-      <c r="E81" s="104" t="s">
+      <c r="E81" s="98" t="s">
         <v>159</v>
       </c>
-      <c r="F81" s="104"/>
-      <c r="G81" s="104"/>
-      <c r="H81" s="104"/>
-      <c r="I81" s="104"/>
-      <c r="J81" s="104"/>
-      <c r="K81" s="104"/>
-      <c r="L81" s="104"/>
-      <c r="M81" s="104"/>
-      <c r="N81" s="104"/>
-      <c r="O81" s="104"/>
-      <c r="P81" s="104" t="s">
+      <c r="F81" s="98"/>
+      <c r="G81" s="98"/>
+      <c r="H81" s="98"/>
+      <c r="I81" s="98"/>
+      <c r="J81" s="98"/>
+      <c r="K81" s="98"/>
+      <c r="L81" s="98"/>
+      <c r="M81" s="98"/>
+      <c r="N81" s="98"/>
+      <c r="O81" s="98"/>
+      <c r="P81" s="98" t="s">
         <v>164</v>
       </c>
-      <c r="Q81" s="104"/>
-      <c r="R81" s="104"/>
-      <c r="S81" s="104"/>
-      <c r="T81" s="104"/>
-      <c r="U81" s="104"/>
-      <c r="V81" s="104"/>
-      <c r="W81" s="104"/>
-      <c r="X81" s="104"/>
-      <c r="Y81" s="104"/>
-      <c r="Z81" s="104"/>
+      <c r="Q81" s="98"/>
+      <c r="R81" s="98"/>
+      <c r="S81" s="98"/>
+      <c r="T81" s="98"/>
+      <c r="U81" s="98"/>
+      <c r="V81" s="98"/>
+      <c r="W81" s="98"/>
+      <c r="X81" s="98"/>
+      <c r="Y81" s="98"/>
+      <c r="Z81" s="98"/>
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A82" s="44" t="s">
@@ -4986,30 +4986,30 @@
       <c r="D82" s="85">
         <v>1</v>
       </c>
-      <c r="E82" s="104" t="s">
+      <c r="E82" s="98" t="s">
         <v>161</v>
       </c>
-      <c r="F82" s="104"/>
-      <c r="G82" s="104"/>
-      <c r="H82" s="104"/>
-      <c r="I82" s="104"/>
-      <c r="J82" s="104"/>
-      <c r="K82" s="104"/>
-      <c r="L82" s="104"/>
-      <c r="M82" s="104"/>
-      <c r="N82" s="104"/>
-      <c r="O82" s="104"/>
-      <c r="P82" s="104"/>
-      <c r="Q82" s="104"/>
-      <c r="R82" s="104"/>
-      <c r="S82" s="104"/>
-      <c r="T82" s="104"/>
-      <c r="U82" s="104"/>
-      <c r="V82" s="104"/>
-      <c r="W82" s="104"/>
-      <c r="X82" s="104"/>
-      <c r="Y82" s="104"/>
-      <c r="Z82" s="104"/>
+      <c r="F82" s="98"/>
+      <c r="G82" s="98"/>
+      <c r="H82" s="98"/>
+      <c r="I82" s="98"/>
+      <c r="J82" s="98"/>
+      <c r="K82" s="98"/>
+      <c r="L82" s="98"/>
+      <c r="M82" s="98"/>
+      <c r="N82" s="98"/>
+      <c r="O82" s="98"/>
+      <c r="P82" s="98"/>
+      <c r="Q82" s="98"/>
+      <c r="R82" s="98"/>
+      <c r="S82" s="98"/>
+      <c r="T82" s="98"/>
+      <c r="U82" s="98"/>
+      <c r="V82" s="98"/>
+      <c r="W82" s="98"/>
+      <c r="X82" s="98"/>
+      <c r="Y82" s="98"/>
+      <c r="Z82" s="98"/>
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A83" s="44" t="s">
@@ -5024,30 +5024,30 @@
       <c r="D83" s="85">
         <v>1</v>
       </c>
-      <c r="E83" s="104" t="s">
+      <c r="E83" s="98" t="s">
         <v>160</v>
       </c>
-      <c r="F83" s="104"/>
-      <c r="G83" s="104"/>
-      <c r="H83" s="104"/>
-      <c r="I83" s="104"/>
-      <c r="J83" s="104"/>
-      <c r="K83" s="104"/>
-      <c r="L83" s="104"/>
-      <c r="M83" s="104"/>
-      <c r="N83" s="104"/>
-      <c r="O83" s="104"/>
-      <c r="P83" s="104"/>
-      <c r="Q83" s="104"/>
-      <c r="R83" s="104"/>
-      <c r="S83" s="104"/>
-      <c r="T83" s="104"/>
-      <c r="U83" s="104"/>
-      <c r="V83" s="104"/>
-      <c r="W83" s="104"/>
-      <c r="X83" s="104"/>
-      <c r="Y83" s="104"/>
-      <c r="Z83" s="104"/>
+      <c r="F83" s="98"/>
+      <c r="G83" s="98"/>
+      <c r="H83" s="98"/>
+      <c r="I83" s="98"/>
+      <c r="J83" s="98"/>
+      <c r="K83" s="98"/>
+      <c r="L83" s="98"/>
+      <c r="M83" s="98"/>
+      <c r="N83" s="98"/>
+      <c r="O83" s="98"/>
+      <c r="P83" s="98"/>
+      <c r="Q83" s="98"/>
+      <c r="R83" s="98"/>
+      <c r="S83" s="98"/>
+      <c r="T83" s="98"/>
+      <c r="U83" s="98"/>
+      <c r="V83" s="98"/>
+      <c r="W83" s="98"/>
+      <c r="X83" s="98"/>
+      <c r="Y83" s="98"/>
+      <c r="Z83" s="98"/>
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A84" s="44" t="s">
@@ -5062,117 +5062,93 @@
       <c r="D84" s="85">
         <v>1</v>
       </c>
-      <c r="E84" s="104" t="s">
+      <c r="E84" s="98" t="s">
         <v>162</v>
       </c>
-      <c r="F84" s="104"/>
-      <c r="G84" s="104"/>
-      <c r="H84" s="104"/>
-      <c r="I84" s="104"/>
-      <c r="J84" s="104"/>
-      <c r="K84" s="104"/>
-      <c r="L84" s="104"/>
-      <c r="M84" s="104"/>
-      <c r="N84" s="104"/>
-      <c r="O84" s="104"/>
-      <c r="P84" s="104" t="s">
+      <c r="F84" s="98"/>
+      <c r="G84" s="98"/>
+      <c r="H84" s="98"/>
+      <c r="I84" s="98"/>
+      <c r="J84" s="98"/>
+      <c r="K84" s="98"/>
+      <c r="L84" s="98"/>
+      <c r="M84" s="98"/>
+      <c r="N84" s="98"/>
+      <c r="O84" s="98"/>
+      <c r="P84" s="98" t="s">
         <v>165</v>
       </c>
-      <c r="Q84" s="104"/>
-      <c r="R84" s="104"/>
-      <c r="S84" s="104"/>
-      <c r="T84" s="104"/>
-      <c r="U84" s="104"/>
-      <c r="V84" s="104"/>
-      <c r="W84" s="104"/>
-      <c r="X84" s="104"/>
-      <c r="Y84" s="104"/>
-      <c r="Z84" s="104"/>
+      <c r="Q84" s="98"/>
+      <c r="R84" s="98"/>
+      <c r="S84" s="98"/>
+      <c r="T84" s="98"/>
+      <c r="U84" s="98"/>
+      <c r="V84" s="98"/>
+      <c r="W84" s="98"/>
+      <c r="X84" s="98"/>
+      <c r="Y84" s="98"/>
+      <c r="Z84" s="98"/>
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A85" s="44"/>
       <c r="B85" s="83"/>
       <c r="C85" s="86"/>
       <c r="D85" s="86"/>
-      <c r="E85" s="104"/>
-      <c r="F85" s="104"/>
-      <c r="G85" s="104"/>
-      <c r="H85" s="104"/>
-      <c r="I85" s="104"/>
-      <c r="J85" s="104"/>
-      <c r="K85" s="104"/>
-      <c r="L85" s="104"/>
-      <c r="M85" s="104"/>
-      <c r="N85" s="104"/>
-      <c r="O85" s="104"/>
-      <c r="P85" s="104"/>
-      <c r="Q85" s="104"/>
-      <c r="R85" s="104"/>
-      <c r="S85" s="104"/>
-      <c r="T85" s="104"/>
-      <c r="U85" s="104"/>
-      <c r="V85" s="104"/>
-      <c r="W85" s="104"/>
-      <c r="X85" s="104"/>
-      <c r="Y85" s="104"/>
-      <c r="Z85" s="104"/>
+      <c r="E85" s="98"/>
+      <c r="F85" s="98"/>
+      <c r="G85" s="98"/>
+      <c r="H85" s="98"/>
+      <c r="I85" s="98"/>
+      <c r="J85" s="98"/>
+      <c r="K85" s="98"/>
+      <c r="L85" s="98"/>
+      <c r="M85" s="98"/>
+      <c r="N85" s="98"/>
+      <c r="O85" s="98"/>
+      <c r="P85" s="98"/>
+      <c r="Q85" s="98"/>
+      <c r="R85" s="98"/>
+      <c r="S85" s="98"/>
+      <c r="T85" s="98"/>
+      <c r="U85" s="98"/>
+      <c r="V85" s="98"/>
+      <c r="W85" s="98"/>
+      <c r="X85" s="98"/>
+      <c r="Y85" s="98"/>
+      <c r="Z85" s="98"/>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A86" s="44"/>
       <c r="B86" s="83"/>
       <c r="C86" s="86"/>
       <c r="D86" s="86"/>
-      <c r="E86" s="104"/>
-      <c r="F86" s="104"/>
-      <c r="G86" s="104"/>
-      <c r="H86" s="104"/>
-      <c r="I86" s="104"/>
-      <c r="J86" s="104"/>
-      <c r="K86" s="104"/>
-      <c r="L86" s="104"/>
-      <c r="M86" s="104"/>
-      <c r="N86" s="104"/>
-      <c r="O86" s="104"/>
-      <c r="P86" s="104"/>
-      <c r="Q86" s="104"/>
-      <c r="R86" s="104"/>
-      <c r="S86" s="104"/>
-      <c r="T86" s="104"/>
-      <c r="U86" s="104"/>
-      <c r="V86" s="104"/>
-      <c r="W86" s="104"/>
-      <c r="X86" s="104"/>
-      <c r="Y86" s="104"/>
-      <c r="Z86" s="104"/>
+      <c r="E86" s="98"/>
+      <c r="F86" s="98"/>
+      <c r="G86" s="98"/>
+      <c r="H86" s="98"/>
+      <c r="I86" s="98"/>
+      <c r="J86" s="98"/>
+      <c r="K86" s="98"/>
+      <c r="L86" s="98"/>
+      <c r="M86" s="98"/>
+      <c r="N86" s="98"/>
+      <c r="O86" s="98"/>
+      <c r="P86" s="98"/>
+      <c r="Q86" s="98"/>
+      <c r="R86" s="98"/>
+      <c r="S86" s="98"/>
+      <c r="T86" s="98"/>
+      <c r="U86" s="98"/>
+      <c r="V86" s="98"/>
+      <c r="W86" s="98"/>
+      <c r="X86" s="98"/>
+      <c r="Y86" s="98"/>
+      <c r="Z86" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="P85:Z85"/>
-    <mergeCell ref="P86:Z86"/>
-    <mergeCell ref="P80:Z80"/>
-    <mergeCell ref="P81:Z81"/>
-    <mergeCell ref="P82:Z82"/>
-    <mergeCell ref="P83:Z83"/>
-    <mergeCell ref="P84:Z84"/>
-    <mergeCell ref="E82:O82"/>
-    <mergeCell ref="E83:O83"/>
-    <mergeCell ref="E84:O84"/>
-    <mergeCell ref="E85:O85"/>
-    <mergeCell ref="E86:O86"/>
-    <mergeCell ref="K74:N74"/>
-    <mergeCell ref="K75:N75"/>
-    <mergeCell ref="K76:N76"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="E76:F76"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="G75:H75"/>
-    <mergeCell ref="G76:H76"/>
-    <mergeCell ref="T67:U67"/>
-    <mergeCell ref="T68:U68"/>
-    <mergeCell ref="T66:U66"/>
-    <mergeCell ref="T69:U69"/>
-    <mergeCell ref="T70:U70"/>
+    <mergeCell ref="E80:O80"/>
+    <mergeCell ref="E81:O81"/>
     <mergeCell ref="N62:R62"/>
     <mergeCell ref="I62:J62"/>
     <mergeCell ref="AF60:AI60"/>
@@ -5185,8 +5161,32 @@
     <mergeCell ref="T63:U63"/>
     <mergeCell ref="T64:U64"/>
     <mergeCell ref="T65:U65"/>
-    <mergeCell ref="E80:O80"/>
-    <mergeCell ref="E81:O81"/>
+    <mergeCell ref="T67:U67"/>
+    <mergeCell ref="T68:U68"/>
+    <mergeCell ref="T66:U66"/>
+    <mergeCell ref="T69:U69"/>
+    <mergeCell ref="T70:U70"/>
+    <mergeCell ref="K74:N74"/>
+    <mergeCell ref="K75:N75"/>
+    <mergeCell ref="K76:N76"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="G76:H76"/>
+    <mergeCell ref="E82:O82"/>
+    <mergeCell ref="E83:O83"/>
+    <mergeCell ref="E84:O84"/>
+    <mergeCell ref="E85:O85"/>
+    <mergeCell ref="E86:O86"/>
+    <mergeCell ref="P85:Z85"/>
+    <mergeCell ref="P86:Z86"/>
+    <mergeCell ref="P80:Z80"/>
+    <mergeCell ref="P81:Z81"/>
+    <mergeCell ref="P82:Z82"/>
+    <mergeCell ref="P83:Z83"/>
+    <mergeCell ref="P84:Z84"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Advanced sound effects: Aircraft NOTE: vehicle sound effect made the game laggy, so I got it off...
</commit_message>
<xml_diff>
--- a/gun infos.xlsx
+++ b/gun infos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4736A8-A927-4A70-97A0-DAE8254FC5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6CF79C-8B6C-4B03-8AD8-F5318474D03A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2860" yWindow="9360" windowWidth="33240" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="172">
   <si>
     <t>Weapon info</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -726,12 +726,36 @@
     <t>When players are within the pickup range near the initial location and not in a house, and not riding a vehicle</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>flare gun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30 ~ 320</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Not reloadable. Shoots upto player's cursor location with maximum distance fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>you cannot fire before fire rate is passed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>red, green, yellow, white</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unkillable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1005,6 +1029,15 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="25">
     <fill>
@@ -1193,7 +1226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1477,6 +1510,11 @@
     <xf numFmtId="0" fontId="16" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1759,8 +1797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1775,6 +1813,9 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="F1" s="106" t="s">
+        <v>169</v>
+      </c>
       <c r="L1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2175,11 +2216,11 @@
         <v>0.5</v>
       </c>
       <c r="P6" s="23">
-        <f t="shared" ref="P6" si="4">-(FLOOR(G6/6,1)-1)</f>
+        <f t="shared" ref="P6:P7" si="4">-(FLOOR(G6/6,1)-1)</f>
         <v>-2</v>
       </c>
       <c r="Q6" s="23">
-        <f t="shared" ref="Q6" si="5">ROUND(C6/G6,3)</f>
+        <f t="shared" ref="Q6:Q7" si="5">ROUND(C6/G6,3)</f>
         <v>0.33300000000000002</v>
       </c>
       <c r="R6" s="37" t="s">
@@ -2208,30 +2249,70 @@
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A7" s="27"/>
-      <c r="B7" s="82"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
+      <c r="A7" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="105" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" s="72">
+        <v>0</v>
+      </c>
+      <c r="D7" s="72">
+        <v>1</v>
+      </c>
+      <c r="E7" s="72">
+        <v>0</v>
+      </c>
+      <c r="F7" s="72">
+        <v>1000</v>
+      </c>
+      <c r="G7" s="72">
+        <v>3</v>
+      </c>
+      <c r="H7" s="72">
+        <v>1</v>
+      </c>
+      <c r="I7" s="72">
+        <v>1000</v>
+      </c>
+      <c r="J7" s="107" t="s">
+        <v>170</v>
+      </c>
       <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
-      <c r="N7" s="72"/>
-      <c r="O7" s="72"/>
-      <c r="P7" s="72"/>
-      <c r="Q7" s="72"/>
-      <c r="R7" s="72"/>
+      <c r="L7" s="23">
+        <f>ROUND(D7*E7/F7*1000,2)</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="23">
+        <f>ROUND(D7*E7/(F7+I7)*1000,2)</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="23">
+        <f>D7*E7*H7</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="38"/>
+      <c r="P7" s="23">
+        <f t="shared" ref="P7" si="8">-(FLOOR(G7/6,1)-1)</f>
+        <v>1</v>
+      </c>
+      <c r="Q7" s="23">
+        <f t="shared" ref="Q7" si="9">ROUND(C7/G7,3)</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="37" t="s">
+        <v>171</v>
+      </c>
       <c r="S7" s="72"/>
-      <c r="T7" s="72"/>
-      <c r="U7" s="72"/>
-      <c r="V7" s="72"/>
-      <c r="W7" s="72"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="39"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="31"/>
       <c r="X7" s="72"/>
+      <c r="Y7" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A8" s="27"/>
@@ -2398,7 +2479,7 @@
       </c>
       <c r="S11" s="23"/>
       <c r="T11" s="23">
-        <f t="shared" ref="T11" si="8" xml:space="preserve"> D11*E11*9/10</f>
+        <f t="shared" ref="T11" si="10" xml:space="preserve"> D11*E11*9/10</f>
         <v>2.7</v>
       </c>
       <c r="U11" s="34">
@@ -3676,7 +3757,7 @@
       <c r="R33" s="37"/>
       <c r="S33" s="23"/>
       <c r="T33" s="23">
-        <f t="shared" ref="T33:T35" si="9" xml:space="preserve"> D33*E33*9/10</f>
+        <f t="shared" ref="T33:T35" si="11" xml:space="preserve"> D33*E33*9/10</f>
         <v>0.18</v>
       </c>
       <c r="U33" s="39">
@@ -3684,7 +3765,7 @@
         <v>44.44</v>
       </c>
       <c r="V33" s="23">
-        <f t="shared" ref="V33:V34" si="10">D33*(E33-0.2)</f>
+        <f t="shared" ref="V33:V34" si="12">D33*(E33-0.2)</f>
         <v>0</v>
       </c>
       <c r="W33" s="39"/>
@@ -3741,7 +3822,7 @@
       <c r="R34" s="37"/>
       <c r="S34" s="23"/>
       <c r="T34" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.36</v>
       </c>
       <c r="U34" s="39">
@@ -3749,7 +3830,7 @@
         <v>22.22</v>
       </c>
       <c r="V34" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
       <c r="W34" s="39">
@@ -3789,7 +3870,7 @@
       <c r="J35" s="23"/>
       <c r="K35" s="23"/>
       <c r="L35" s="23">
-        <f t="shared" ref="L35" si="11">ROUND(D35*E35/F35*1000,3)</f>
+        <f t="shared" ref="L35" si="13">ROUND(D35*E35/F35*1000,3)</f>
         <v>2</v>
       </c>
       <c r="M35" s="23">
@@ -3806,7 +3887,7 @@
       <c r="R35" s="37"/>
       <c r="S35" s="23"/>
       <c r="T35" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.9</v>
       </c>
       <c r="U35" s="38">
@@ -4072,47 +4153,47 @@
         <v>74</v>
       </c>
       <c r="B53" s="42">
-        <f t="shared" ref="B53:L53" si="12">(2+B52)*tilesize</f>
+        <f t="shared" ref="B53:L53" si="14">(2+B52)*tilesize</f>
         <v>128</v>
       </c>
       <c r="C53" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>256</v>
       </c>
       <c r="D53" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>384</v>
       </c>
       <c r="E53" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>512</v>
       </c>
       <c r="F53" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>640</v>
       </c>
       <c r="G53" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>768</v>
       </c>
       <c r="H53" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>896</v>
       </c>
       <c r="I53" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1024</v>
       </c>
       <c r="J53" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1152</v>
       </c>
       <c r="K53" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1280</v>
       </c>
       <c r="L53" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1408</v>
       </c>
     </row>
@@ -4121,47 +4202,47 @@
         <v>75</v>
       </c>
       <c r="B54" s="53">
-        <f t="shared" ref="B54:L54" si="13">(2+B52+1)*tilesize+tilesize/2</f>
+        <f t="shared" ref="B54:L54" si="15">(2+B52+1)*tilesize+tilesize/2</f>
         <v>320</v>
       </c>
       <c r="C54" s="54">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>448</v>
       </c>
       <c r="D54" s="55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>576</v>
       </c>
       <c r="E54" s="56">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>704</v>
       </c>
       <c r="F54" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>832</v>
       </c>
       <c r="G54" s="58">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>960</v>
       </c>
       <c r="H54" s="59">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1088</v>
       </c>
       <c r="I54" s="60">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1216</v>
       </c>
       <c r="J54" s="61">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1344</v>
       </c>
       <c r="K54" s="62">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1472</v>
       </c>
       <c r="L54" s="63">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1600</v>
       </c>
     </row>
@@ -4236,7 +4317,7 @@
       </c>
       <c r="L62" s="94">
         <f>COUNTIF(G3:G35,"&gt;0")</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N62" s="102" t="s">
         <v>114</v>
@@ -4335,7 +4416,7 @@
         <v>0</v>
       </c>
       <c r="I64" s="86">
-        <f t="shared" ref="I64:I69" si="14">(B64-player_radius)*2</f>
+        <f t="shared" ref="I64:I69" si="16">(B64-player_radius)*2</f>
         <v>16</v>
       </c>
       <c r="J64" s="86"/>
@@ -4349,19 +4430,19 @@
       </c>
       <c r="M64" s="86"/>
       <c r="N64" s="87">
-        <f t="shared" ref="N64:N70" si="15">ROUND(C64/health_cap,2)*10</f>
+        <f t="shared" ref="N64:N70" si="17">ROUND(C64/health_cap,2)*10</f>
         <v>0.8</v>
       </c>
       <c r="O64" s="89">
-        <f t="shared" ref="O64:O70" si="16">ROUND(L64/guns_cap,2)*10</f>
+        <f t="shared" ref="O64:O70" si="18">ROUND(L64/guns_cap,2)*10</f>
         <v>3.3000000000000003</v>
       </c>
       <c r="P64" s="91">
-        <f t="shared" ref="P64:P70" si="17">ROUND(D64/speed_cap,2)*10</f>
+        <f t="shared" ref="P64:P70" si="19">ROUND(D64/speed_cap,2)*10</f>
         <v>6</v>
       </c>
       <c r="Q64" s="88">
-        <f t="shared" ref="Q64:Q70" si="18">ROUND(H64/DPS_cap,2)*10</f>
+        <f t="shared" ref="Q64:Q70" si="20">ROUND(H64/DPS_cap,2)*10</f>
         <v>0</v>
       </c>
       <c r="R64" s="96">
@@ -4407,7 +4488,7 @@
         <v>0</v>
       </c>
       <c r="I65" s="86">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>32</v>
       </c>
       <c r="J65" s="86"/>
@@ -4416,33 +4497,33 @@
         <v>2</v>
       </c>
       <c r="L65" s="86">
-        <f t="shared" ref="L65:L68" si="19">21-K65</f>
+        <f t="shared" ref="L65:L68" si="21">21-K65</f>
         <v>19</v>
       </c>
       <c r="M65" s="86"/>
       <c r="N65" s="87">
-        <f t="shared" si="15"/>
-        <v>3</v>
-      </c>
-      <c r="O65" s="89">
-        <f t="shared" si="16"/>
-        <v>6.3</v>
-      </c>
-      <c r="P65" s="91">
         <f t="shared" si="17"/>
         <v>3</v>
       </c>
+      <c r="O65" s="89">
+        <f t="shared" si="18"/>
+        <v>6.3</v>
+      </c>
+      <c r="P65" s="91">
+        <f t="shared" si="19"/>
+        <v>3</v>
+      </c>
       <c r="Q65" s="88">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R65" s="96">
-        <f t="shared" ref="R65:R69" si="20">SUM(N65:Q65)</f>
+        <f t="shared" ref="R65:R69" si="22">SUM(N65:Q65)</f>
         <v>12.3</v>
       </c>
       <c r="S65" s="86"/>
       <c r="T65" s="101">
-        <f t="shared" ref="T65:T70" si="21">Q65+N65+O65</f>
+        <f t="shared" ref="T65:T70" si="23">Q65+N65+O65</f>
         <v>9.3000000000000007</v>
       </c>
       <c r="U65" s="101"/>
@@ -4479,7 +4560,7 @@
         <v>11.11</v>
       </c>
       <c r="I66" s="86">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>28</v>
       </c>
       <c r="J66" s="86"/>
@@ -4488,33 +4569,33 @@
         <v>4</v>
       </c>
       <c r="L66" s="86">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>17</v>
       </c>
       <c r="M66" s="86"/>
       <c r="N66" s="87">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2.5</v>
       </c>
       <c r="O66" s="89">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>5.6999999999999993</v>
       </c>
       <c r="P66" s="91">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
       <c r="Q66" s="88">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="R66" s="96">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>14.399999999999999</v>
       </c>
       <c r="S66" s="86"/>
       <c r="T66" s="101">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>10.399999999999999</v>
       </c>
       <c r="U66" s="101"/>
@@ -4551,7 +4632,7 @@
         <v>5.63</v>
       </c>
       <c r="I67" s="86">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>48</v>
       </c>
       <c r="J67" s="86"/>
@@ -4560,33 +4641,33 @@
         <v>0</v>
       </c>
       <c r="L67" s="86">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>21</v>
       </c>
       <c r="M67" s="86"/>
       <c r="N67" s="87">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>9.6</v>
       </c>
       <c r="O67" s="89">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>7</v>
       </c>
       <c r="P67" s="91">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="Q67" s="88">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="R67" s="96">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>18.700000000000003</v>
       </c>
       <c r="S67" s="86"/>
       <c r="T67" s="101">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>17.7</v>
       </c>
       <c r="U67" s="101"/>
@@ -4619,7 +4700,7 @@
         <v>13.33</v>
       </c>
       <c r="I68" s="86">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>72</v>
       </c>
       <c r="J68" s="86"/>
@@ -4628,33 +4709,33 @@
         <v>0</v>
       </c>
       <c r="L68" s="86">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>21</v>
       </c>
       <c r="M68" s="86"/>
       <c r="N68" s="87">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>7.4</v>
       </c>
       <c r="O68" s="89">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>7</v>
       </c>
       <c r="P68" s="91">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Q68" s="88">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>2.7</v>
       </c>
       <c r="R68" s="96">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>17.100000000000001</v>
       </c>
       <c r="S68" s="86"/>
       <c r="T68" s="101">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>17.100000000000001</v>
       </c>
       <c r="U68" s="101"/>
@@ -4687,7 +4768,7 @@
         <v>9.09</v>
       </c>
       <c r="I69" s="86">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>20</v>
       </c>
       <c r="J69" s="86"/>
@@ -4701,28 +4782,28 @@
       </c>
       <c r="M69" s="86"/>
       <c r="N69" s="87">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
       <c r="O69" s="89">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="P69" s="91">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
       <c r="Q69" s="88">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>1.7999999999999998</v>
       </c>
       <c r="R69" s="96">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>18.8</v>
       </c>
       <c r="S69" s="86"/>
       <c r="T69" s="101">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>8.8000000000000007</v>
       </c>
       <c r="U69" s="101"/>
@@ -4755,7 +4836,7 @@
         <v>48</v>
       </c>
       <c r="I70" s="86">
-        <f t="shared" ref="I70" si="22">(B70-player_radius)*2</f>
+        <f t="shared" ref="I70" si="24">(B70-player_radius)*2</f>
         <v>24</v>
       </c>
       <c r="J70" s="86"/>
@@ -4769,28 +4850,28 @@
       </c>
       <c r="M70" s="86"/>
       <c r="N70" s="87">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2.5</v>
       </c>
       <c r="O70" s="89">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>5.6999999999999993</v>
       </c>
       <c r="P70" s="91">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
       <c r="Q70" s="88">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>9.6</v>
       </c>
       <c r="R70" s="96">
-        <f t="shared" ref="R70" si="23">SUM(N70:Q70)</f>
+        <f t="shared" ref="R70" si="25">SUM(N70:Q70)</f>
         <v>25.799999999999997</v>
       </c>
       <c r="S70" s="86"/>
       <c r="T70" s="101">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>17.799999999999997</v>
       </c>
       <c r="U70" s="101"/>

</xml_diff>